<commit_message>
Backup before Ubuntu reinstall
</commit_message>
<xml_diff>
--- a/16-Bit Computer Manual v2.xlsx
+++ b/16-Bit Computer Manual v2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="895">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2021" uniqueCount="957">
   <si>
     <t xml:space="preserve">ADDRESS</t>
   </si>
@@ -2581,9 +2581,90 @@
     <t xml:space="preserve">rA15 := imm</t>
   </si>
   <si>
+    <t xml:space="preserve">TOKENS/OP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arity: 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arity: 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arity: 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x0037</t>
   </si>
   <si>
+    <t xml:space="preserve">IFETCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEWLINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRINT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRINTSTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUSH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JZ/JE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JNZ/JNE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOVF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JLE/JNG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JL/JNGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XCHG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUB(R/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIV(R/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S(A/H)(R/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EQU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RES</t>
+  </si>
+  <si>
     <t xml:space="preserve">CALL imm II</t>
   </si>
   <si>
@@ -2593,121 +2674,226 @@
     <t xml:space="preserve">0x0038</t>
   </si>
   <si>
+    <t xml:space="preserve">AccessLabel</t>
+  </si>
+  <si>
     <t xml:space="preserve">CALL imm III</t>
   </si>
   <si>
+    <t xml:space="preserve">AccessLabelWithIndex</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x0039</t>
   </si>
   <si>
+    <t xml:space="preserve">Array</t>
+  </si>
+  <si>
     <t xml:space="preserve">CALL imm IV</t>
   </si>
   <si>
+    <t xml:space="preserve">EntryLabel</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x003A</t>
   </si>
   <si>
+    <t xml:space="preserve">IntegerExpression</t>
+  </si>
+  <si>
     <t xml:space="preserve">CALL imm V</t>
   </si>
   <si>
     <t xml:space="preserve">PC = DBUS</t>
   </si>
   <si>
+    <t xml:space="preserve">JumpLabel</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x003B</t>
   </si>
   <si>
+    <t xml:space="preserve">NameLiteral</t>
+  </si>
+  <si>
     <t xml:space="preserve">RET I </t>
   </si>
   <si>
+    <t xml:space="preserve">Operator</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x003C</t>
   </si>
   <si>
+    <t xml:space="preserve">RegistryAccess</t>
+  </si>
+  <si>
     <t xml:space="preserve">RET II</t>
   </si>
   <si>
+    <t xml:space="preserve">StringLiteral</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x003D</t>
   </si>
   <si>
+    <t xml:space="preserve">AccLab | AccLab</t>
+  </si>
+  <si>
     <t xml:space="preserve">RET III</t>
   </si>
   <si>
     <t xml:space="preserve">DBUS -&gt; PC</t>
   </si>
   <si>
+    <t xml:space="preserve">AccLab | ALWIndex</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x003E</t>
   </si>
   <si>
+    <t xml:space="preserve">AccLab | Array</t>
+  </si>
+  <si>
     <t xml:space="preserve">RET IV</t>
   </si>
   <si>
+    <t xml:space="preserve">AccLab | EntryL</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x003F</t>
   </si>
   <si>
+    <t xml:space="preserve">AccLab | IntExp</t>
+  </si>
+  <si>
     <t xml:space="preserve">PRINT RB I </t>
   </si>
   <si>
     <t xml:space="preserve">RB := RB + 0 (for translating the result over ALU)</t>
   </si>
   <si>
+    <t xml:space="preserve">AccLab | JmpL</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x0040</t>
   </si>
   <si>
+    <t xml:space="preserve">AccLab | NameL</t>
+  </si>
+  <si>
     <t xml:space="preserve">MOV ESP, EBP I </t>
   </si>
   <si>
+    <t xml:space="preserve">AccLab | OP</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x0041</t>
   </si>
   <si>
+    <t xml:space="preserve">AccLab | RegAcc</t>
+  </si>
+  <si>
     <t xml:space="preserve">MOV ESP, EBP II</t>
   </si>
   <si>
     <t xml:space="preserve">rB15 -&gt; DBUS</t>
   </si>
   <si>
+    <t xml:space="preserve">AccLab | StringL</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x0042</t>
   </si>
   <si>
+    <t xml:space="preserve">ALWIndex | AccLab</t>
+  </si>
+  <si>
     <t xml:space="preserve">MOV EBP, ESP I </t>
   </si>
   <si>
+    <t xml:space="preserve">ALWIndex | ALWIndex</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x0043</t>
   </si>
   <si>
+    <t xml:space="preserve">ALWIndex | Array</t>
+  </si>
+  <si>
     <t xml:space="preserve">MOV EBP, ESP II</t>
   </si>
   <si>
     <t xml:space="preserve">DBUS -&gt; EBP</t>
   </si>
   <si>
+    <t xml:space="preserve">ALWIndex | EntryL</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x0044</t>
   </si>
   <si>
+    <t xml:space="preserve">ALWIndex | IntExp</t>
+  </si>
+  <si>
     <t xml:space="preserve">PUSH EBP I </t>
   </si>
   <si>
+    <t xml:space="preserve">ALWIndex | JmpL</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x0045</t>
   </si>
   <si>
+    <t xml:space="preserve">ALWIndex | NameL</t>
+  </si>
+  <si>
     <t xml:space="preserve">PUSH EBP II</t>
   </si>
   <si>
+    <t xml:space="preserve">ALWIndex | OP</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x0046</t>
   </si>
   <si>
+    <t xml:space="preserve">ALWIndex | RegAcc</t>
+  </si>
+  <si>
     <t xml:space="preserve">PUSH EBP III</t>
   </si>
   <si>
+    <t xml:space="preserve">ALWIndex | StringL</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x0047</t>
   </si>
   <si>
+    <t xml:space="preserve">Array | AccLab</t>
+  </si>
+  <si>
     <t xml:space="preserve">PUSH EBP IV</t>
   </si>
   <si>
+    <t xml:space="preserve">Array | ALWIndex</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x0048</t>
   </si>
   <si>
+    <t xml:space="preserve">Array | Array</t>
+  </si>
+  <si>
     <t xml:space="preserve">POP EBP I </t>
   </si>
   <si>
+    <t xml:space="preserve">Array | EntryL</t>
+  </si>
+  <si>
     <t xml:space="preserve">0x0049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Array | IntExp</t>
   </si>
   <si>
     <t xml:space="preserve">POP EBP II</t>
@@ -3083,7 +3269,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3239,8 +3425,22 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3250,13 +3450,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF63838"/>
-        <bgColor rgb="FFFF6600"/>
+        <bgColor rgb="FFED1C24"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor rgb="FF70AD47"/>
+        <bgColor rgb="FF72BF44"/>
       </patternFill>
     </fill>
     <fill>
@@ -3268,35 +3468,59 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
-        <bgColor rgb="FF33CCCC"/>
+        <bgColor rgb="FF00B6BD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFAA61A"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFED1C24"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF70AD47"/>
+        <bgColor rgb="FF72BF44"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
         <bgColor rgb="FFF63838"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF70AD47"/>
-        <bgColor rgb="FF92D050"/>
+        <fgColor rgb="FF00B6BD"/>
+        <bgColor rgb="FF00B0F0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF6600"/>
-        <bgColor rgb="FFFF9900"/>
+        <fgColor rgb="FFFAA61A"/>
+        <bgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF72BF44"/>
+        <bgColor rgb="FF70AD47"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED1C24"/>
+        <bgColor rgb="FFF63838"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="82">
+  <borders count="98">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -3865,10 +4089,122 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="dashed"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom style="dashed"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="dashed"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dashed"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dashed"/>
+      <right style="dashed"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="dashed"/>
+      <top/>
+      <bottom style="dashed"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dashed"/>
+      <right style="dashed"/>
+      <top/>
+      <bottom style="dashed"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dashed"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="dashed"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="dashed"/>
+      <top style="dashed"/>
+      <bottom style="dashed"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dashed"/>
+      <right style="dashed"/>
+      <top style="dashed"/>
+      <bottom style="dashed"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dashed"/>
+      <right style="thin"/>
+      <top style="dashed"/>
+      <bottom style="dashed"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin"/>
       <top style="mediumDashDot"/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="dashed"/>
+      <top style="dashed"/>
+      <bottom style="double"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dashed"/>
+      <right style="dashed"/>
+      <top style="dashed"/>
+      <bottom style="double"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dashed"/>
+      <right style="thin"/>
+      <top style="dashed"/>
+      <bottom style="double"/>
       <diagonal/>
     </border>
   </borders>
@@ -3897,7 +4233,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="209">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4583,7 +4919,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="72" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="22" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="22" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="5" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -4646,11 +4982,91 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="81" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="10" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="10" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="81" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="82" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="83" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="84" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="85" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="86" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="87" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="88" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="89" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="90" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="91" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="92" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="93" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="94" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="95" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="96" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="97" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="94" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4665,12 +5081,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
     </dxf>
   </dxfs>
   <colors>
@@ -4716,18 +5127,18 @@
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF00B6BD"/>
       <rgbColor rgb="FF92D050"/>
       <rgbColor rgb="FFFFC000"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFAA61A"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF70AD47"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF72BF44"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFED1C24"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -4743,8 +5154,8 @@
   </sheetPr>
   <dimension ref="A1:EL246"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CI1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CM3" activeCellId="0" sqref="CM3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4752,8 +5163,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="11.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="87" min="4" style="1" width="4.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="117" min="88" style="1" width="11.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="129" min="118" style="1" width="4.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="130" style="1" width="11.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="121" min="118" style="1" width="11.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="129" min="122" style="1" width="4.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="134" min="130" style="1" width="4.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="135" style="1" width="11.78"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -34354,10 +34767,57 @@
         <f aca="false">IF(CI120=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ119" s="8" t="s">
+        <v>730</v>
+      </c>
+      <c r="CR119" s="8"/>
+      <c r="CS119" s="8"/>
+      <c r="CT119" s="170" t="s">
+        <v>731</v>
+      </c>
+      <c r="CU119" s="170"/>
+      <c r="CV119" s="170"/>
+      <c r="CW119" s="170" t="s">
+        <v>732</v>
+      </c>
+      <c r="CX119" s="170"/>
+      <c r="CY119" s="170"/>
+      <c r="CZ119" s="170"/>
+      <c r="DA119" s="170"/>
+      <c r="DB119" s="170"/>
+      <c r="DC119" s="170"/>
+      <c r="DD119" s="170"/>
+      <c r="DE119" s="170"/>
+      <c r="DF119" s="170"/>
+      <c r="DG119" s="170"/>
+      <c r="DH119" s="170"/>
+      <c r="DI119" s="170"/>
+      <c r="DJ119" s="170" t="s">
+        <v>733</v>
+      </c>
+      <c r="DK119" s="170"/>
+      <c r="DL119" s="170"/>
+      <c r="DM119" s="170"/>
+      <c r="DN119" s="170"/>
+      <c r="DO119" s="170"/>
+      <c r="DP119" s="170"/>
+      <c r="DQ119" s="170"/>
+      <c r="DR119" s="170"/>
+      <c r="DS119" s="170"/>
+      <c r="DT119" s="170"/>
+      <c r="DU119" s="170"/>
+      <c r="DV119" s="170"/>
+      <c r="DW119" s="170"/>
+      <c r="DX119" s="170"/>
+      <c r="DY119" s="170"/>
+      <c r="DZ119" s="170"/>
+      <c r="EA119" s="170"/>
+      <c r="EB119" s="170"/>
+      <c r="EC119" s="170"/>
     </row>
     <row r="120" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="109" t="s">
-        <v>730</v>
+        <v>734</v>
       </c>
       <c r="B120" s="109"/>
       <c r="C120" s="109"/>
@@ -34613,10 +35073,109 @@
       <c r="CI120" s="51" t="n">
         <v>0</v>
       </c>
+      <c r="CQ120" s="8"/>
+      <c r="CR120" s="8"/>
+      <c r="CS120" s="8"/>
+      <c r="CT120" s="187" t="s">
+        <v>28</v>
+      </c>
+      <c r="CU120" s="187" t="s">
+        <v>735</v>
+      </c>
+      <c r="CV120" s="187" t="s">
+        <v>736</v>
+      </c>
+      <c r="CW120" s="187" t="s">
+        <v>737</v>
+      </c>
+      <c r="CX120" s="188" t="s">
+        <v>738</v>
+      </c>
+      <c r="CY120" s="187" t="s">
+        <v>739</v>
+      </c>
+      <c r="CZ120" s="187" t="s">
+        <v>740</v>
+      </c>
+      <c r="DA120" s="187" t="s">
+        <v>741</v>
+      </c>
+      <c r="DB120" s="187" t="s">
+        <v>716</v>
+      </c>
+      <c r="DC120" s="187" t="s">
+        <v>742</v>
+      </c>
+      <c r="DD120" s="187" t="s">
+        <v>743</v>
+      </c>
+      <c r="DE120" s="187" t="s">
+        <v>744</v>
+      </c>
+      <c r="DF120" s="187" t="s">
+        <v>745</v>
+      </c>
+      <c r="DG120" s="187" t="s">
+        <v>746</v>
+      </c>
+      <c r="DH120" s="187" t="s">
+        <v>747</v>
+      </c>
+      <c r="DI120" s="187" t="s">
+        <v>748</v>
+      </c>
+      <c r="DJ120" s="187" t="s">
+        <v>749</v>
+      </c>
+      <c r="DK120" s="187" t="s">
+        <v>750</v>
+      </c>
+      <c r="DL120" s="187" t="s">
+        <v>687</v>
+      </c>
+      <c r="DM120" s="187" t="s">
+        <v>697</v>
+      </c>
+      <c r="DN120" s="188" t="s">
+        <v>751</v>
+      </c>
+      <c r="DO120" s="188" t="s">
+        <v>752</v>
+      </c>
+      <c r="DP120" s="189" t="s">
+        <v>753</v>
+      </c>
+      <c r="DQ120" s="187" t="s">
+        <v>712</v>
+      </c>
+      <c r="DR120" s="190" t="s">
+        <v>707</v>
+      </c>
+      <c r="DS120" s="190"/>
+      <c r="DT120" s="191" t="s">
+        <v>754</v>
+      </c>
+      <c r="DU120" s="191"/>
+      <c r="DV120" s="191" t="s">
+        <v>124</v>
+      </c>
+      <c r="DW120" s="191"/>
+      <c r="DX120" s="190" t="s">
+        <v>755</v>
+      </c>
+      <c r="DY120" s="190"/>
+      <c r="DZ120" s="190" t="s">
+        <v>756</v>
+      </c>
+      <c r="EA120" s="190"/>
+      <c r="EB120" s="190" t="s">
+        <v>757</v>
+      </c>
+      <c r="EC120" s="190"/>
     </row>
     <row r="121" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="186" t="s">
-        <v>731</v>
+        <v>758</v>
       </c>
       <c r="B121" s="186"/>
       <c r="C121" s="186"/>
@@ -34628,7 +35187,7 @@
       <c r="G121" s="92"/>
       <c r="H121" s="92"/>
       <c r="I121" s="93" t="s">
-        <v>732</v>
+        <v>759</v>
       </c>
       <c r="J121" s="93"/>
       <c r="K121" s="93"/>
@@ -34722,10 +35281,18 @@
         <f aca="false">IF(CI122=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ121" s="192" t="s">
+        <v>569</v>
+      </c>
+      <c r="CR121" s="192"/>
+      <c r="CS121" s="192"/>
+      <c r="CT121" s="193"/>
+      <c r="CU121" s="194"/>
+      <c r="CV121" s="195"/>
     </row>
     <row r="122" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="109" t="s">
-        <v>733</v>
+        <v>760</v>
       </c>
       <c r="B122" s="109"/>
       <c r="C122" s="109"/>
@@ -34981,10 +35548,18 @@
       <c r="CI122" s="51" t="n">
         <v>0</v>
       </c>
+      <c r="CQ122" s="192" t="s">
+        <v>761</v>
+      </c>
+      <c r="CR122" s="192"/>
+      <c r="CS122" s="192"/>
+      <c r="CT122" s="196"/>
+      <c r="CU122" s="197"/>
+      <c r="CV122" s="198"/>
     </row>
     <row r="123" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="186" t="s">
-        <v>734</v>
+        <v>762</v>
       </c>
       <c r="B123" s="186"/>
       <c r="C123" s="186"/>
@@ -35090,10 +35665,18 @@
         <f aca="false">IF(CI124=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ123" s="192" t="s">
+        <v>763</v>
+      </c>
+      <c r="CR123" s="192"/>
+      <c r="CS123" s="192"/>
+      <c r="CT123" s="199"/>
+      <c r="CU123" s="200"/>
+      <c r="CV123" s="201"/>
     </row>
     <row r="124" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="109" t="s">
-        <v>735</v>
+        <v>764</v>
       </c>
       <c r="B124" s="109"/>
       <c r="C124" s="109"/>
@@ -35349,10 +35932,18 @@
       <c r="CI124" s="51" t="n">
         <v>0</v>
       </c>
+      <c r="CQ124" s="192" t="s">
+        <v>765</v>
+      </c>
+      <c r="CR124" s="192"/>
+      <c r="CS124" s="192"/>
+      <c r="CT124" s="199"/>
+      <c r="CU124" s="200"/>
+      <c r="CV124" s="201"/>
     </row>
     <row r="125" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="186" t="s">
-        <v>736</v>
+        <v>766</v>
       </c>
       <c r="B125" s="186"/>
       <c r="C125" s="186"/>
@@ -35458,10 +36049,18 @@
         <f aca="false">IF(CI126=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ125" s="192" t="s">
+        <v>767</v>
+      </c>
+      <c r="CR125" s="192"/>
+      <c r="CS125" s="192"/>
+      <c r="CT125" s="199"/>
+      <c r="CU125" s="200"/>
+      <c r="CV125" s="201"/>
     </row>
     <row r="126" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="109" t="s">
-        <v>737</v>
+        <v>768</v>
       </c>
       <c r="B126" s="109"/>
       <c r="C126" s="109"/>
@@ -35717,10 +36316,18 @@
       <c r="CI126" s="51" t="n">
         <v>0</v>
       </c>
+      <c r="CQ126" s="192" t="s">
+        <v>769</v>
+      </c>
+      <c r="CR126" s="192"/>
+      <c r="CS126" s="192"/>
+      <c r="CT126" s="199"/>
+      <c r="CU126" s="200"/>
+      <c r="CV126" s="201"/>
     </row>
     <row r="127" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="186" t="s">
-        <v>738</v>
+        <v>770</v>
       </c>
       <c r="B127" s="186"/>
       <c r="C127" s="186"/>
@@ -35732,7 +36339,7 @@
       <c r="G127" s="92"/>
       <c r="H127" s="92"/>
       <c r="I127" s="93" t="s">
-        <v>739</v>
+        <v>771</v>
       </c>
       <c r="J127" s="93"/>
       <c r="K127" s="93"/>
@@ -35826,10 +36433,18 @@
         <f aca="false">IF(CI128=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ127" s="192" t="s">
+        <v>772</v>
+      </c>
+      <c r="CR127" s="192"/>
+      <c r="CS127" s="192"/>
+      <c r="CT127" s="199"/>
+      <c r="CU127" s="200"/>
+      <c r="CV127" s="201"/>
     </row>
     <row r="128" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="80" t="s">
-        <v>740</v>
+        <v>773</v>
       </c>
       <c r="B128" s="80"/>
       <c r="C128" s="80"/>
@@ -36085,10 +36700,18 @@
       <c r="CI128" s="87" t="n">
         <v>0</v>
       </c>
+      <c r="CQ128" s="192" t="s">
+        <v>774</v>
+      </c>
+      <c r="CR128" s="192"/>
+      <c r="CS128" s="192"/>
+      <c r="CT128" s="199"/>
+      <c r="CU128" s="200"/>
+      <c r="CV128" s="201"/>
     </row>
     <row r="129" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="186" t="s">
-        <v>741</v>
+        <v>775</v>
       </c>
       <c r="B129" s="186"/>
       <c r="C129" s="186"/>
@@ -36178,14 +36801,14 @@
       <c r="BY129" s="93"/>
       <c r="BZ129" s="93"/>
       <c r="CA129" s="93"/>
-      <c r="CB129" s="187" t="s">
+      <c r="CB129" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC129" s="187"/>
-      <c r="CD129" s="187"/>
-      <c r="CE129" s="187"/>
-      <c r="CF129" s="187"/>
-      <c r="CG129" s="187"/>
+      <c r="CC129" s="202"/>
+      <c r="CD129" s="202"/>
+      <c r="CE129" s="202"/>
+      <c r="CF129" s="202"/>
+      <c r="CG129" s="202"/>
       <c r="CH129" s="93" t="str">
         <f aca="false">IF(CH130=0,"-", "+")</f>
         <v>+</v>
@@ -36194,10 +36817,18 @@
         <f aca="false">IF(CI130=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ129" s="192" t="s">
+        <v>776</v>
+      </c>
+      <c r="CR129" s="192"/>
+      <c r="CS129" s="192"/>
+      <c r="CT129" s="199"/>
+      <c r="CU129" s="200"/>
+      <c r="CV129" s="201"/>
     </row>
     <row r="130" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="109" t="s">
-        <v>742</v>
+        <v>777</v>
       </c>
       <c r="B130" s="109"/>
       <c r="C130" s="109"/>
@@ -36453,10 +37084,18 @@
       <c r="CI130" s="51" t="n">
         <v>0</v>
       </c>
+      <c r="CQ130" s="192" t="s">
+        <v>778</v>
+      </c>
+      <c r="CR130" s="192"/>
+      <c r="CS130" s="192"/>
+      <c r="CT130" s="199"/>
+      <c r="CU130" s="200"/>
+      <c r="CV130" s="201"/>
     </row>
     <row r="131" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="186" t="s">
-        <v>743</v>
+        <v>779</v>
       </c>
       <c r="B131" s="186"/>
       <c r="C131" s="186"/>
@@ -36562,10 +37201,18 @@
         <f aca="false">IF(CI132=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ131" s="203" t="s">
+        <v>780</v>
+      </c>
+      <c r="CR131" s="203"/>
+      <c r="CS131" s="203"/>
+      <c r="CT131" s="204"/>
+      <c r="CU131" s="205"/>
+      <c r="CV131" s="206"/>
     </row>
     <row r="132" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="109" t="s">
-        <v>744</v>
+        <v>781</v>
       </c>
       <c r="B132" s="109"/>
       <c r="C132" s="109"/>
@@ -36821,10 +37468,15 @@
       <c r="CI132" s="51" t="n">
         <v>0</v>
       </c>
+      <c r="CQ132" s="192" t="s">
+        <v>782</v>
+      </c>
+      <c r="CR132" s="192"/>
+      <c r="CS132" s="192"/>
     </row>
     <row r="133" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="186" t="s">
-        <v>745</v>
+        <v>783</v>
       </c>
       <c r="B133" s="186"/>
       <c r="C133" s="186"/>
@@ -36836,7 +37488,7 @@
       <c r="G133" s="92"/>
       <c r="H133" s="92"/>
       <c r="I133" s="93" t="s">
-        <v>746</v>
+        <v>784</v>
       </c>
       <c r="J133" s="93"/>
       <c r="K133" s="93"/>
@@ -36930,10 +37582,15 @@
         <f aca="false">IF(CI134=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ133" s="192" t="s">
+        <v>785</v>
+      </c>
+      <c r="CR133" s="192"/>
+      <c r="CS133" s="192"/>
     </row>
     <row r="134" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="109" t="s">
-        <v>747</v>
+        <v>786</v>
       </c>
       <c r="B134" s="109"/>
       <c r="C134" s="109"/>
@@ -37189,10 +37846,15 @@
       <c r="CI134" s="51" t="n">
         <v>0</v>
       </c>
+      <c r="CQ134" s="192" t="s">
+        <v>787</v>
+      </c>
+      <c r="CR134" s="192"/>
+      <c r="CS134" s="192"/>
     </row>
     <row r="135" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="186" t="s">
-        <v>748</v>
+        <v>788</v>
       </c>
       <c r="B135" s="186"/>
       <c r="C135" s="186"/>
@@ -37298,10 +37960,15 @@
         <f aca="false">IF(CI136=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ135" s="192" t="s">
+        <v>789</v>
+      </c>
+      <c r="CR135" s="192"/>
+      <c r="CS135" s="192"/>
     </row>
     <row r="136" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="80" t="s">
-        <v>749</v>
+        <v>790</v>
       </c>
       <c r="B136" s="80"/>
       <c r="C136" s="80"/>
@@ -37557,10 +38224,15 @@
       <c r="CI136" s="87" t="n">
         <v>0</v>
       </c>
+      <c r="CQ136" s="192" t="s">
+        <v>791</v>
+      </c>
+      <c r="CR136" s="192"/>
+      <c r="CS136" s="192"/>
     </row>
     <row r="137" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="91" t="s">
-        <v>750</v>
+        <v>792</v>
       </c>
       <c r="B137" s="91"/>
       <c r="C137" s="91"/>
@@ -37609,7 +38281,7 @@
       <c r="AL137" s="93"/>
       <c r="AM137" s="93"/>
       <c r="AN137" s="93" t="s">
-        <v>751</v>
+        <v>793</v>
       </c>
       <c r="AO137" s="93"/>
       <c r="AP137" s="93"/>
@@ -37666,10 +38338,15 @@
         <f aca="false">IF(CI138=0,"-", "+")</f>
         <v>+</v>
       </c>
+      <c r="CQ137" s="192" t="s">
+        <v>794</v>
+      </c>
+      <c r="CR137" s="192"/>
+      <c r="CS137" s="192"/>
     </row>
     <row r="138" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="80" t="s">
-        <v>752</v>
+        <v>795</v>
       </c>
       <c r="B138" s="80"/>
       <c r="C138" s="80"/>
@@ -37925,13 +38602,18 @@
       <c r="CI138" s="87" t="n">
         <v>1</v>
       </c>
+      <c r="CQ138" s="192" t="s">
+        <v>796</v>
+      </c>
+      <c r="CR138" s="192"/>
+      <c r="CS138" s="192"/>
     </row>
     <row r="139" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A139" s="188" t="s">
-        <v>753</v>
-      </c>
-      <c r="B139" s="188"/>
-      <c r="C139" s="188"/>
+      <c r="A139" s="207" t="s">
+        <v>797</v>
+      </c>
+      <c r="B139" s="207"/>
+      <c r="C139" s="207"/>
       <c r="D139" s="92" t="s">
         <v>408</v>
       </c>
@@ -38034,10 +38716,15 @@
         <f aca="false">IF(CI140=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ139" s="192" t="s">
+        <v>798</v>
+      </c>
+      <c r="CR139" s="192"/>
+      <c r="CS139" s="192"/>
     </row>
     <row r="140" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="109" t="s">
-        <v>754</v>
+        <v>799</v>
       </c>
       <c r="B140" s="109"/>
       <c r="C140" s="109"/>
@@ -38293,10 +38980,15 @@
       <c r="CI140" s="51" t="n">
         <v>0</v>
       </c>
+      <c r="CQ140" s="192" t="s">
+        <v>800</v>
+      </c>
+      <c r="CR140" s="192"/>
+      <c r="CS140" s="192"/>
     </row>
     <row r="141" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="13" t="s">
-        <v>755</v>
+        <v>801</v>
       </c>
       <c r="B141" s="13"/>
       <c r="C141" s="13"/>
@@ -38345,7 +39037,7 @@
       <c r="AL141" s="93"/>
       <c r="AM141" s="93"/>
       <c r="AN141" s="93" t="s">
-        <v>756</v>
+        <v>802</v>
       </c>
       <c r="AO141" s="93"/>
       <c r="AP141" s="93"/>
@@ -38402,10 +39094,18 @@
         <f aca="false">IF(CI142=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ141" s="203" t="s">
+        <v>803</v>
+      </c>
+      <c r="CR141" s="203"/>
+      <c r="CS141" s="203"/>
+      <c r="CT141" s="208"/>
+      <c r="CU141" s="208"/>
+      <c r="CV141" s="208"/>
     </row>
     <row r="142" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="80" t="s">
-        <v>757</v>
+        <v>804</v>
       </c>
       <c r="B142" s="80"/>
       <c r="C142" s="80"/>
@@ -38661,10 +39361,15 @@
       <c r="CI142" s="87" t="n">
         <v>0</v>
       </c>
+      <c r="CQ142" s="192" t="s">
+        <v>805</v>
+      </c>
+      <c r="CR142" s="192"/>
+      <c r="CS142" s="192"/>
     </row>
     <row r="143" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="13" t="s">
-        <v>758</v>
+        <v>806</v>
       </c>
       <c r="B143" s="13"/>
       <c r="C143" s="13"/>
@@ -38754,14 +39459,14 @@
       <c r="BY143" s="93"/>
       <c r="BZ143" s="93"/>
       <c r="CA143" s="93"/>
-      <c r="CB143" s="187" t="s">
+      <c r="CB143" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC143" s="187"/>
-      <c r="CD143" s="187"/>
-      <c r="CE143" s="187"/>
-      <c r="CF143" s="187"/>
-      <c r="CG143" s="187"/>
+      <c r="CC143" s="202"/>
+      <c r="CD143" s="202"/>
+      <c r="CE143" s="202"/>
+      <c r="CF143" s="202"/>
+      <c r="CG143" s="202"/>
       <c r="CH143" s="93" t="str">
         <f aca="false">IF(CH144=0,"-", "+")</f>
         <v>+</v>
@@ -38770,10 +39475,15 @@
         <f aca="false">IF(CI144=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ143" s="192" t="s">
+        <v>807</v>
+      </c>
+      <c r="CR143" s="192"/>
+      <c r="CS143" s="192"/>
     </row>
     <row r="144" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="109" t="s">
-        <v>759</v>
+        <v>808</v>
       </c>
       <c r="B144" s="109"/>
       <c r="C144" s="109"/>
@@ -39029,15 +39739,20 @@
       <c r="CI144" s="51" t="n">
         <v>0</v>
       </c>
+      <c r="CQ144" s="192" t="s">
+        <v>809</v>
+      </c>
+      <c r="CR144" s="192"/>
+      <c r="CS144" s="192"/>
     </row>
     <row r="145" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="13" t="s">
-        <v>760</v>
+        <v>810</v>
       </c>
       <c r="B145" s="13"/>
       <c r="C145" s="13"/>
       <c r="D145" s="92" t="s">
-        <v>761</v>
+        <v>811</v>
       </c>
       <c r="E145" s="92"/>
       <c r="F145" s="92"/>
@@ -39081,7 +39796,7 @@
       <c r="AL145" s="93"/>
       <c r="AM145" s="93"/>
       <c r="AN145" s="93" t="s">
-        <v>756</v>
+        <v>802</v>
       </c>
       <c r="AO145" s="93"/>
       <c r="AP145" s="93"/>
@@ -39138,10 +39853,15 @@
         <f aca="false">IF(CI146=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ145" s="192" t="s">
+        <v>812</v>
+      </c>
+      <c r="CR145" s="192"/>
+      <c r="CS145" s="192"/>
     </row>
     <row r="146" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="80" t="s">
-        <v>762</v>
+        <v>813</v>
       </c>
       <c r="B146" s="80"/>
       <c r="C146" s="80"/>
@@ -39397,13 +40117,18 @@
       <c r="CI146" s="87" t="n">
         <v>0</v>
       </c>
+      <c r="CQ146" s="192" t="s">
+        <v>814</v>
+      </c>
+      <c r="CR146" s="192"/>
+      <c r="CS146" s="192"/>
     </row>
     <row r="147" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A147" s="188" t="s">
-        <v>763</v>
-      </c>
-      <c r="B147" s="188"/>
-      <c r="C147" s="188"/>
+      <c r="A147" s="207" t="s">
+        <v>815</v>
+      </c>
+      <c r="B147" s="207"/>
+      <c r="C147" s="207"/>
       <c r="D147" s="92" t="s">
         <v>408</v>
       </c>
@@ -39506,10 +40231,15 @@
         <f aca="false">IF(CI148=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ147" s="192" t="s">
+        <v>816</v>
+      </c>
+      <c r="CR147" s="192"/>
+      <c r="CS147" s="192"/>
     </row>
     <row r="148" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="109" t="s">
-        <v>764</v>
+        <v>817</v>
       </c>
       <c r="B148" s="109"/>
       <c r="C148" s="109"/>
@@ -39765,10 +40495,15 @@
       <c r="CI148" s="51" t="n">
         <v>0</v>
       </c>
+      <c r="CQ148" s="192" t="s">
+        <v>818</v>
+      </c>
+      <c r="CR148" s="192"/>
+      <c r="CS148" s="192"/>
     </row>
     <row r="149" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="13" t="s">
-        <v>765</v>
+        <v>819</v>
       </c>
       <c r="B149" s="13"/>
       <c r="C149" s="13"/>
@@ -39817,7 +40552,7 @@
       <c r="AL149" s="93"/>
       <c r="AM149" s="93"/>
       <c r="AN149" s="93" t="s">
-        <v>756</v>
+        <v>802</v>
       </c>
       <c r="AO149" s="93"/>
       <c r="AP149" s="93"/>
@@ -39874,10 +40609,15 @@
         <f aca="false">IF(CI150=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ149" s="192" t="s">
+        <v>820</v>
+      </c>
+      <c r="CR149" s="192"/>
+      <c r="CS149" s="192"/>
     </row>
     <row r="150" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="109" t="s">
-        <v>766</v>
+        <v>821</v>
       </c>
       <c r="B150" s="109"/>
       <c r="C150" s="109"/>
@@ -40133,10 +40873,15 @@
       <c r="CI150" s="51" t="n">
         <v>0</v>
       </c>
+      <c r="CQ150" s="192" t="s">
+        <v>822</v>
+      </c>
+      <c r="CR150" s="192"/>
+      <c r="CS150" s="192"/>
     </row>
     <row r="151" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="13" t="s">
-        <v>767</v>
+        <v>823</v>
       </c>
       <c r="B151" s="13"/>
       <c r="C151" s="13"/>
@@ -40242,10 +40987,18 @@
         <f aca="false">IF(CI152=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ151" s="203" t="s">
+        <v>824</v>
+      </c>
+      <c r="CR151" s="203"/>
+      <c r="CS151" s="203"/>
+      <c r="CT151" s="208"/>
+      <c r="CU151" s="208"/>
+      <c r="CV151" s="208"/>
     </row>
     <row r="152" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="109" t="s">
-        <v>768</v>
+        <v>825</v>
       </c>
       <c r="B152" s="109"/>
       <c r="C152" s="109"/>
@@ -40501,10 +41254,15 @@
       <c r="CI152" s="51" t="n">
         <v>0</v>
       </c>
+      <c r="CQ152" s="192" t="s">
+        <v>826</v>
+      </c>
+      <c r="CR152" s="192"/>
+      <c r="CS152" s="192"/>
     </row>
     <row r="153" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="13" t="s">
-        <v>769</v>
+        <v>827</v>
       </c>
       <c r="B153" s="13"/>
       <c r="C153" s="13"/>
@@ -40610,10 +41368,15 @@
         <f aca="false">IF(CI154=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ153" s="192" t="s">
+        <v>828</v>
+      </c>
+      <c r="CR153" s="192"/>
+      <c r="CS153" s="192"/>
     </row>
     <row r="154" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="80" t="s">
-        <v>770</v>
+        <v>829</v>
       </c>
       <c r="B154" s="80"/>
       <c r="C154" s="80"/>
@@ -40869,13 +41632,18 @@
       <c r="CI154" s="87" t="n">
         <v>0</v>
       </c>
+      <c r="CQ154" s="192" t="s">
+        <v>830</v>
+      </c>
+      <c r="CR154" s="192"/>
+      <c r="CS154" s="192"/>
     </row>
     <row r="155" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A155" s="188" t="s">
-        <v>771</v>
-      </c>
-      <c r="B155" s="188"/>
-      <c r="C155" s="188"/>
+      <c r="A155" s="207" t="s">
+        <v>831</v>
+      </c>
+      <c r="B155" s="207"/>
+      <c r="C155" s="207"/>
       <c r="D155" s="92" t="s">
         <v>290</v>
       </c>
@@ -40978,10 +41746,15 @@
         <f aca="false">IF(CI156=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ155" s="192" t="s">
+        <v>832</v>
+      </c>
+      <c r="CR155" s="192"/>
+      <c r="CS155" s="192"/>
     </row>
     <row r="156" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="109" t="s">
-        <v>772</v>
+        <v>833</v>
       </c>
       <c r="B156" s="109"/>
       <c r="C156" s="109"/>
@@ -41237,10 +42010,15 @@
       <c r="CI156" s="51" t="n">
         <v>0</v>
       </c>
+      <c r="CQ156" s="192" t="s">
+        <v>834</v>
+      </c>
+      <c r="CR156" s="192"/>
+      <c r="CS156" s="192"/>
     </row>
     <row r="157" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="13" t="s">
-        <v>773</v>
+        <v>835</v>
       </c>
       <c r="B157" s="13"/>
       <c r="C157" s="13"/>
@@ -41349,7 +42127,7 @@
     </row>
     <row r="158" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="109" t="s">
-        <v>774</v>
+        <v>836</v>
       </c>
       <c r="B158" s="109"/>
       <c r="C158" s="109"/>
@@ -41608,7 +42386,7 @@
     </row>
     <row r="159" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="13" t="s">
-        <v>775</v>
+        <v>837</v>
       </c>
       <c r="B159" s="13"/>
       <c r="C159" s="13"/>
@@ -41717,7 +42495,7 @@
     </row>
     <row r="160" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="109" t="s">
-        <v>776</v>
+        <v>838</v>
       </c>
       <c r="B160" s="109"/>
       <c r="C160" s="109"/>
@@ -41976,12 +42754,12 @@
     </row>
     <row r="161" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="13" t="s">
-        <v>777</v>
+        <v>839</v>
       </c>
       <c r="B161" s="13"/>
       <c r="C161" s="13"/>
       <c r="D161" s="92" t="s">
-        <v>761</v>
+        <v>811</v>
       </c>
       <c r="E161" s="92"/>
       <c r="F161" s="92"/>
@@ -42025,7 +42803,7 @@
       <c r="AL161" s="93"/>
       <c r="AM161" s="93"/>
       <c r="AN161" s="93" t="s">
-        <v>756</v>
+        <v>802</v>
       </c>
       <c r="AO161" s="93"/>
       <c r="AP161" s="93"/>
@@ -42085,7 +42863,7 @@
     </row>
     <row r="162" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="80" t="s">
-        <v>778</v>
+        <v>840</v>
       </c>
       <c r="B162" s="80"/>
       <c r="C162" s="80"/>
@@ -42343,11 +43121,11 @@
       </c>
     </row>
     <row r="163" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A163" s="188" t="s">
-        <v>779</v>
-      </c>
-      <c r="B163" s="188"/>
-      <c r="C163" s="188"/>
+      <c r="A163" s="207" t="s">
+        <v>841</v>
+      </c>
+      <c r="B163" s="207"/>
+      <c r="C163" s="207"/>
       <c r="D163" s="92" t="s">
         <v>150</v>
       </c>
@@ -42453,7 +43231,7 @@
     </row>
     <row r="164" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="109" t="s">
-        <v>780</v>
+        <v>842</v>
       </c>
       <c r="B164" s="109"/>
       <c r="C164" s="109"/>
@@ -42712,7 +43490,7 @@
     </row>
     <row r="165" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="13" t="s">
-        <v>781</v>
+        <v>843</v>
       </c>
       <c r="B165" s="13"/>
       <c r="C165" s="13"/>
@@ -42753,7 +43531,7 @@
       <c r="AF165" s="93"/>
       <c r="AG165" s="93"/>
       <c r="AH165" s="93" t="s">
-        <v>782</v>
+        <v>844</v>
       </c>
       <c r="AI165" s="93"/>
       <c r="AJ165" s="93"/>
@@ -42761,7 +43539,7 @@
       <c r="AL165" s="93"/>
       <c r="AM165" s="93"/>
       <c r="AN165" s="93" t="s">
-        <v>783</v>
+        <v>845</v>
       </c>
       <c r="AO165" s="93"/>
       <c r="AP165" s="93"/>
@@ -42821,7 +43599,7 @@
     </row>
     <row r="166" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="109" t="s">
-        <v>784</v>
+        <v>846</v>
       </c>
       <c r="B166" s="109"/>
       <c r="C166" s="109"/>
@@ -43080,7 +43858,7 @@
     </row>
     <row r="167" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="13" t="s">
-        <v>785</v>
+        <v>847</v>
       </c>
       <c r="B167" s="13"/>
       <c r="C167" s="13"/>
@@ -43189,7 +43967,7 @@
     </row>
     <row r="168" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="80" t="s">
-        <v>786</v>
+        <v>848</v>
       </c>
       <c r="B168" s="80"/>
       <c r="C168" s="80"/>
@@ -43447,11 +44225,11 @@
       </c>
     </row>
     <row r="169" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A169" s="188" t="s">
-        <v>787</v>
-      </c>
-      <c r="B169" s="188"/>
-      <c r="C169" s="188"/>
+      <c r="A169" s="207" t="s">
+        <v>849</v>
+      </c>
+      <c r="B169" s="207"/>
+      <c r="C169" s="207"/>
       <c r="D169" s="92" t="s">
         <v>290</v>
       </c>
@@ -43538,14 +44316,14 @@
       <c r="BY169" s="93"/>
       <c r="BZ169" s="93"/>
       <c r="CA169" s="93"/>
-      <c r="CB169" s="187" t="s">
+      <c r="CB169" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC169" s="187"/>
-      <c r="CD169" s="187"/>
-      <c r="CE169" s="187"/>
-      <c r="CF169" s="187"/>
-      <c r="CG169" s="187"/>
+      <c r="CC169" s="202"/>
+      <c r="CD169" s="202"/>
+      <c r="CE169" s="202"/>
+      <c r="CF169" s="202"/>
+      <c r="CG169" s="202"/>
       <c r="CH169" s="93" t="str">
         <f aca="false">IF(CH170=0,"-", "+")</f>
         <v>+</v>
@@ -43557,7 +44335,7 @@
     </row>
     <row r="170" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="109" t="s">
-        <v>788</v>
+        <v>850</v>
       </c>
       <c r="B170" s="109"/>
       <c r="C170" s="109"/>
@@ -43816,7 +44594,7 @@
     </row>
     <row r="171" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="13" t="s">
-        <v>789</v>
+        <v>851</v>
       </c>
       <c r="B171" s="13"/>
       <c r="C171" s="13"/>
@@ -43857,7 +44635,7 @@
       <c r="AF171" s="93"/>
       <c r="AG171" s="93"/>
       <c r="AH171" s="93" t="s">
-        <v>782</v>
+        <v>844</v>
       </c>
       <c r="AI171" s="93"/>
       <c r="AJ171" s="93"/>
@@ -43865,7 +44643,7 @@
       <c r="AL171" s="93"/>
       <c r="AM171" s="93"/>
       <c r="AN171" s="93" t="s">
-        <v>790</v>
+        <v>852</v>
       </c>
       <c r="AO171" s="93"/>
       <c r="AP171" s="93"/>
@@ -43925,7 +44703,7 @@
     </row>
     <row r="172" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="109" t="s">
-        <v>791</v>
+        <v>853</v>
       </c>
       <c r="B172" s="109"/>
       <c r="C172" s="109"/>
@@ -44184,7 +44962,7 @@
     </row>
     <row r="173" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="13" t="s">
-        <v>792</v>
+        <v>854</v>
       </c>
       <c r="B173" s="13"/>
       <c r="C173" s="13"/>
@@ -44293,7 +45071,7 @@
     </row>
     <row r="174" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="80" t="s">
-        <v>793</v>
+        <v>855</v>
       </c>
       <c r="B174" s="80"/>
       <c r="C174" s="80"/>
@@ -44553,7 +45331,7 @@
     </row>
     <row r="175" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="91" t="s">
-        <v>794</v>
+        <v>856</v>
       </c>
       <c r="B175" s="91"/>
       <c r="C175" s="91"/>
@@ -44573,7 +45351,7 @@
       <c r="M175" s="93"/>
       <c r="N175" s="93"/>
       <c r="O175" s="93" t="s">
-        <v>795</v>
+        <v>857</v>
       </c>
       <c r="P175" s="93"/>
       <c r="Q175" s="93"/>
@@ -44594,7 +45372,7 @@
       <c r="AF175" s="93"/>
       <c r="AG175" s="93"/>
       <c r="AH175" s="93" t="s">
-        <v>796</v>
+        <v>858</v>
       </c>
       <c r="AI175" s="93"/>
       <c r="AJ175" s="93"/>
@@ -44643,14 +45421,14 @@
       <c r="BY175" s="93"/>
       <c r="BZ175" s="93"/>
       <c r="CA175" s="93"/>
-      <c r="CB175" s="187" t="s">
+      <c r="CB175" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC175" s="187"/>
-      <c r="CD175" s="187"/>
-      <c r="CE175" s="187"/>
-      <c r="CF175" s="187"/>
-      <c r="CG175" s="187"/>
+      <c r="CC175" s="202"/>
+      <c r="CD175" s="202"/>
+      <c r="CE175" s="202"/>
+      <c r="CF175" s="202"/>
+      <c r="CG175" s="202"/>
       <c r="CH175" s="93" t="str">
         <f aca="false">IF(CH176=0,"-", "+")</f>
         <v>-</v>
@@ -44663,7 +45441,7 @@
     </row>
     <row r="176" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="109" t="s">
-        <v>797</v>
+        <v>859</v>
       </c>
       <c r="B176" s="109"/>
       <c r="C176" s="109"/>
@@ -44923,7 +45701,7 @@
     </row>
     <row r="177" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="91" t="s">
-        <v>798</v>
+        <v>860</v>
       </c>
       <c r="B177" s="91"/>
       <c r="C177" s="91"/>
@@ -45040,7 +45818,7 @@
     </row>
     <row r="178" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="109" t="s">
-        <v>799</v>
+        <v>861</v>
       </c>
       <c r="B178" s="109"/>
       <c r="C178" s="109"/>
@@ -45306,7 +46084,7 @@
     </row>
     <row r="179" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="91" t="s">
-        <v>800</v>
+        <v>862</v>
       </c>
       <c r="B179" s="91"/>
       <c r="C179" s="91"/>
@@ -45415,7 +46193,7 @@
     </row>
     <row r="180" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="80" t="s">
-        <v>801</v>
+        <v>863</v>
       </c>
       <c r="B180" s="80"/>
       <c r="C180" s="80"/>
@@ -45674,7 +46452,7 @@
     </row>
     <row r="181" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="91" t="s">
-        <v>802</v>
+        <v>864</v>
       </c>
       <c r="B181" s="91"/>
       <c r="C181" s="91"/>
@@ -45694,7 +46472,7 @@
       <c r="M181" s="93"/>
       <c r="N181" s="93"/>
       <c r="O181" s="93" t="s">
-        <v>803</v>
+        <v>865</v>
       </c>
       <c r="P181" s="93"/>
       <c r="Q181" s="93"/>
@@ -45715,7 +46493,7 @@
       <c r="AF181" s="93"/>
       <c r="AG181" s="93"/>
       <c r="AH181" s="93" t="s">
-        <v>804</v>
+        <v>866</v>
       </c>
       <c r="AI181" s="93"/>
       <c r="AJ181" s="93"/>
@@ -45764,14 +46542,14 @@
       <c r="BY181" s="93"/>
       <c r="BZ181" s="93"/>
       <c r="CA181" s="93"/>
-      <c r="CB181" s="187" t="s">
+      <c r="CB181" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC181" s="187"/>
-      <c r="CD181" s="187"/>
-      <c r="CE181" s="187"/>
-      <c r="CF181" s="187"/>
-      <c r="CG181" s="187"/>
+      <c r="CC181" s="202"/>
+      <c r="CD181" s="202"/>
+      <c r="CE181" s="202"/>
+      <c r="CF181" s="202"/>
+      <c r="CG181" s="202"/>
       <c r="CH181" s="93" t="str">
         <f aca="false">IF(CH182=0,"-", "+")</f>
         <v>-</v>
@@ -45783,7 +46561,7 @@
     </row>
     <row r="182" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="109" t="s">
-        <v>805</v>
+        <v>867</v>
       </c>
       <c r="B182" s="109"/>
       <c r="C182" s="109"/>
@@ -46042,7 +46820,7 @@
     </row>
     <row r="183" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="91" t="s">
-        <v>806</v>
+        <v>868</v>
       </c>
       <c r="B183" s="91"/>
       <c r="C183" s="91"/>
@@ -46151,7 +46929,7 @@
     </row>
     <row r="184" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="109" t="s">
-        <v>807</v>
+        <v>869</v>
       </c>
       <c r="B184" s="109"/>
       <c r="C184" s="109"/>
@@ -46410,7 +47188,7 @@
     </row>
     <row r="185" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="91" t="s">
-        <v>808</v>
+        <v>870</v>
       </c>
       <c r="B185" s="91"/>
       <c r="C185" s="91"/>
@@ -46519,7 +47297,7 @@
     </row>
     <row r="186" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="80" t="s">
-        <v>809</v>
+        <v>871</v>
       </c>
       <c r="B186" s="80"/>
       <c r="C186" s="80"/>
@@ -46778,7 +47556,7 @@
     </row>
     <row r="187" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="91" t="s">
-        <v>810</v>
+        <v>872</v>
       </c>
       <c r="B187" s="91"/>
       <c r="C187" s="91"/>
@@ -46798,7 +47576,7 @@
       <c r="M187" s="93"/>
       <c r="N187" s="93"/>
       <c r="O187" s="93" t="s">
-        <v>811</v>
+        <v>873</v>
       </c>
       <c r="P187" s="93"/>
       <c r="Q187" s="93"/>
@@ -46819,7 +47597,7 @@
       <c r="AF187" s="93"/>
       <c r="AG187" s="93"/>
       <c r="AH187" s="93" t="s">
-        <v>812</v>
+        <v>874</v>
       </c>
       <c r="AI187" s="93"/>
       <c r="AJ187" s="93"/>
@@ -46868,14 +47646,14 @@
       <c r="BY187" s="93"/>
       <c r="BZ187" s="93"/>
       <c r="CA187" s="93"/>
-      <c r="CB187" s="187" t="s">
+      <c r="CB187" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC187" s="187"/>
-      <c r="CD187" s="187"/>
-      <c r="CE187" s="187"/>
-      <c r="CF187" s="187"/>
-      <c r="CG187" s="187"/>
+      <c r="CC187" s="202"/>
+      <c r="CD187" s="202"/>
+      <c r="CE187" s="202"/>
+      <c r="CF187" s="202"/>
+      <c r="CG187" s="202"/>
       <c r="CH187" s="93" t="str">
         <f aca="false">IF(CH188=0,"-", "+")</f>
         <v>-</v>
@@ -46887,7 +47665,7 @@
     </row>
     <row r="188" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="109" t="s">
-        <v>813</v>
+        <v>875</v>
       </c>
       <c r="B188" s="109"/>
       <c r="C188" s="109"/>
@@ -47146,7 +47924,7 @@
     </row>
     <row r="189" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="91" t="s">
-        <v>814</v>
+        <v>876</v>
       </c>
       <c r="B189" s="91"/>
       <c r="C189" s="91"/>
@@ -47255,7 +48033,7 @@
     </row>
     <row r="190" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="109" t="s">
-        <v>815</v>
+        <v>877</v>
       </c>
       <c r="B190" s="109"/>
       <c r="C190" s="109"/>
@@ -47514,7 +48292,7 @@
     </row>
     <row r="191" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="91" t="s">
-        <v>816</v>
+        <v>878</v>
       </c>
       <c r="B191" s="91"/>
       <c r="C191" s="91"/>
@@ -47623,7 +48401,7 @@
     </row>
     <row r="192" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="80" t="s">
-        <v>817</v>
+        <v>879</v>
       </c>
       <c r="B192" s="80"/>
       <c r="C192" s="80"/>
@@ -47882,7 +48660,7 @@
     </row>
     <row r="193" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="91" t="s">
-        <v>818</v>
+        <v>880</v>
       </c>
       <c r="B193" s="91"/>
       <c r="C193" s="91"/>
@@ -47902,7 +48680,7 @@
       <c r="M193" s="93"/>
       <c r="N193" s="93"/>
       <c r="O193" s="93" t="s">
-        <v>819</v>
+        <v>881</v>
       </c>
       <c r="P193" s="93"/>
       <c r="Q193" s="93"/>
@@ -47923,7 +48701,7 @@
       <c r="AF193" s="93"/>
       <c r="AG193" s="93"/>
       <c r="AH193" s="93" t="s">
-        <v>820</v>
+        <v>882</v>
       </c>
       <c r="AI193" s="93"/>
       <c r="AJ193" s="93"/>
@@ -47972,14 +48750,14 @@
       <c r="BY193" s="93"/>
       <c r="BZ193" s="93"/>
       <c r="CA193" s="93"/>
-      <c r="CB193" s="187" t="s">
+      <c r="CB193" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC193" s="187"/>
-      <c r="CD193" s="187"/>
-      <c r="CE193" s="187"/>
-      <c r="CF193" s="187"/>
-      <c r="CG193" s="187"/>
+      <c r="CC193" s="202"/>
+      <c r="CD193" s="202"/>
+      <c r="CE193" s="202"/>
+      <c r="CF193" s="202"/>
+      <c r="CG193" s="202"/>
       <c r="CH193" s="93" t="str">
         <f aca="false">IF(CH194=0,"-", "+")</f>
         <v>-</v>
@@ -47991,7 +48769,7 @@
     </row>
     <row r="194" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="109" t="s">
-        <v>821</v>
+        <v>883</v>
       </c>
       <c r="B194" s="109"/>
       <c r="C194" s="109"/>
@@ -48250,7 +49028,7 @@
     </row>
     <row r="195" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="91" t="s">
-        <v>822</v>
+        <v>884</v>
       </c>
       <c r="B195" s="91"/>
       <c r="C195" s="91"/>
@@ -48359,7 +49137,7 @@
     </row>
     <row r="196" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="109" t="s">
-        <v>823</v>
+        <v>885</v>
       </c>
       <c r="B196" s="109"/>
       <c r="C196" s="109"/>
@@ -48618,7 +49396,7 @@
     </row>
     <row r="197" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="91" t="s">
-        <v>824</v>
+        <v>886</v>
       </c>
       <c r="B197" s="91"/>
       <c r="C197" s="91"/>
@@ -48727,7 +49505,7 @@
     </row>
     <row r="198" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="80" t="s">
-        <v>825</v>
+        <v>887</v>
       </c>
       <c r="B198" s="80"/>
       <c r="C198" s="80"/>
@@ -48985,11 +49763,11 @@
       </c>
     </row>
     <row r="199" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A199" s="188" t="s">
-        <v>826</v>
-      </c>
-      <c r="B199" s="188"/>
-      <c r="C199" s="188"/>
+      <c r="A199" s="207" t="s">
+        <v>888</v>
+      </c>
+      <c r="B199" s="207"/>
+      <c r="C199" s="207"/>
       <c r="D199" s="92" t="s">
         <v>150</v>
       </c>
@@ -49035,7 +49813,7 @@
       <c r="AL199" s="93"/>
       <c r="AM199" s="93"/>
       <c r="AN199" s="93" t="s">
-        <v>827</v>
+        <v>889</v>
       </c>
       <c r="AO199" s="93"/>
       <c r="AP199" s="93"/>
@@ -49076,14 +49854,14 @@
       <c r="BY199" s="93"/>
       <c r="BZ199" s="93"/>
       <c r="CA199" s="93"/>
-      <c r="CB199" s="187" t="s">
+      <c r="CB199" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC199" s="187"/>
-      <c r="CD199" s="187"/>
-      <c r="CE199" s="187"/>
-      <c r="CF199" s="187"/>
-      <c r="CG199" s="187"/>
+      <c r="CC199" s="202"/>
+      <c r="CD199" s="202"/>
+      <c r="CE199" s="202"/>
+      <c r="CF199" s="202"/>
+      <c r="CG199" s="202"/>
       <c r="CH199" s="93" t="str">
         <f aca="false">IF(CH200=0,"-", "+")</f>
         <v>+</v>
@@ -49095,7 +49873,7 @@
     </row>
     <row r="200" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="80" t="s">
-        <v>828</v>
+        <v>890</v>
       </c>
       <c r="B200" s="80"/>
       <c r="C200" s="80"/>
@@ -49353,11 +50131,11 @@
       </c>
     </row>
     <row r="201" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A201" s="188" t="s">
-        <v>829</v>
-      </c>
-      <c r="B201" s="188"/>
-      <c r="C201" s="188"/>
+      <c r="A201" s="207" t="s">
+        <v>891</v>
+      </c>
+      <c r="B201" s="207"/>
+      <c r="C201" s="207"/>
       <c r="D201" s="92" t="s">
         <v>150</v>
       </c>
@@ -49403,7 +50181,7 @@
       <c r="AL201" s="93"/>
       <c r="AM201" s="93"/>
       <c r="AN201" s="93" t="s">
-        <v>830</v>
+        <v>892</v>
       </c>
       <c r="AO201" s="93"/>
       <c r="AP201" s="93"/>
@@ -49444,14 +50222,14 @@
       <c r="BY201" s="93"/>
       <c r="BZ201" s="93"/>
       <c r="CA201" s="93"/>
-      <c r="CB201" s="187" t="s">
+      <c r="CB201" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC201" s="187"/>
-      <c r="CD201" s="187"/>
-      <c r="CE201" s="187"/>
-      <c r="CF201" s="187"/>
-      <c r="CG201" s="187"/>
+      <c r="CC201" s="202"/>
+      <c r="CD201" s="202"/>
+      <c r="CE201" s="202"/>
+      <c r="CF201" s="202"/>
+      <c r="CG201" s="202"/>
       <c r="CH201" s="93" t="str">
         <f aca="false">IF(CH202=0,"-", "+")</f>
         <v>+</v>
@@ -49463,7 +50241,7 @@
     </row>
     <row r="202" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="80" t="s">
-        <v>831</v>
+        <v>893</v>
       </c>
       <c r="B202" s="80"/>
       <c r="C202" s="80"/>
@@ -49722,7 +50500,7 @@
     </row>
     <row r="203" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="91" t="s">
-        <v>832</v>
+        <v>894</v>
       </c>
       <c r="B203" s="91"/>
       <c r="C203" s="91"/>
@@ -49771,7 +50549,7 @@
       <c r="AL203" s="93"/>
       <c r="AM203" s="93"/>
       <c r="AN203" s="93" t="s">
-        <v>833</v>
+        <v>895</v>
       </c>
       <c r="AO203" s="93"/>
       <c r="AP203" s="93"/>
@@ -49812,14 +50590,14 @@
       <c r="BY203" s="93"/>
       <c r="BZ203" s="93"/>
       <c r="CA203" s="93"/>
-      <c r="CB203" s="187" t="s">
+      <c r="CB203" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC203" s="187"/>
-      <c r="CD203" s="187"/>
-      <c r="CE203" s="187"/>
-      <c r="CF203" s="187"/>
-      <c r="CG203" s="187"/>
+      <c r="CC203" s="202"/>
+      <c r="CD203" s="202"/>
+      <c r="CE203" s="202"/>
+      <c r="CF203" s="202"/>
+      <c r="CG203" s="202"/>
       <c r="CH203" s="93" t="str">
         <f aca="false">IF(CH204=0,"-", "+")</f>
         <v>+</v>
@@ -49831,7 +50609,7 @@
     </row>
     <row r="204" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="80" t="s">
-        <v>834</v>
+        <v>896</v>
       </c>
       <c r="B204" s="80"/>
       <c r="C204" s="80"/>
@@ -50090,7 +50868,7 @@
     </row>
     <row r="205" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="91" t="s">
-        <v>835</v>
+        <v>897</v>
       </c>
       <c r="B205" s="91"/>
       <c r="C205" s="91"/>
@@ -50139,7 +50917,7 @@
       <c r="AL205" s="93"/>
       <c r="AM205" s="93"/>
       <c r="AN205" s="93" t="s">
-        <v>836</v>
+        <v>898</v>
       </c>
       <c r="AO205" s="93"/>
       <c r="AP205" s="93"/>
@@ -50180,14 +50958,14 @@
       <c r="BY205" s="93"/>
       <c r="BZ205" s="93"/>
       <c r="CA205" s="93"/>
-      <c r="CB205" s="187" t="s">
+      <c r="CB205" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC205" s="187"/>
-      <c r="CD205" s="187"/>
-      <c r="CE205" s="187"/>
-      <c r="CF205" s="187"/>
-      <c r="CG205" s="187"/>
+      <c r="CC205" s="202"/>
+      <c r="CD205" s="202"/>
+      <c r="CE205" s="202"/>
+      <c r="CF205" s="202"/>
+      <c r="CG205" s="202"/>
       <c r="CH205" s="93" t="str">
         <f aca="false">IF(CH206=0,"-", "+")</f>
         <v>+</v>
@@ -50199,7 +50977,7 @@
     </row>
     <row r="206" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="80" t="s">
-        <v>837</v>
+        <v>899</v>
       </c>
       <c r="B206" s="80"/>
       <c r="C206" s="80"/>
@@ -50457,11 +51235,11 @@
       </c>
     </row>
     <row r="207" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A207" s="188" t="s">
-        <v>838</v>
-      </c>
-      <c r="B207" s="188"/>
-      <c r="C207" s="188"/>
+      <c r="A207" s="207" t="s">
+        <v>900</v>
+      </c>
+      <c r="B207" s="207"/>
+      <c r="C207" s="207"/>
       <c r="D207" s="92" t="s">
         <v>166</v>
       </c>
@@ -50507,7 +51285,7 @@
       <c r="AL207" s="93"/>
       <c r="AM207" s="93"/>
       <c r="AN207" s="93" t="s">
-        <v>839</v>
+        <v>901</v>
       </c>
       <c r="AO207" s="93"/>
       <c r="AP207" s="93"/>
@@ -50548,14 +51326,14 @@
       <c r="BY207" s="93"/>
       <c r="BZ207" s="93"/>
       <c r="CA207" s="93"/>
-      <c r="CB207" s="187" t="s">
+      <c r="CB207" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC207" s="187"/>
-      <c r="CD207" s="187"/>
-      <c r="CE207" s="187"/>
-      <c r="CF207" s="187"/>
-      <c r="CG207" s="187"/>
+      <c r="CC207" s="202"/>
+      <c r="CD207" s="202"/>
+      <c r="CE207" s="202"/>
+      <c r="CF207" s="202"/>
+      <c r="CG207" s="202"/>
       <c r="CH207" s="93" t="str">
         <f aca="false">IF(CH208=0,"-", "+")</f>
         <v>-</v>
@@ -50567,7 +51345,7 @@
     </row>
     <row r="208" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A208" s="109" t="s">
-        <v>840</v>
+        <v>902</v>
       </c>
       <c r="B208" s="109"/>
       <c r="C208" s="109"/>
@@ -50826,7 +51604,7 @@
     </row>
     <row r="209" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="13" t="s">
-        <v>841</v>
+        <v>903</v>
       </c>
       <c r="B209" s="13"/>
       <c r="C209" s="13"/>
@@ -50935,7 +51713,7 @@
     </row>
     <row r="210" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="109" t="s">
-        <v>842</v>
+        <v>904</v>
       </c>
       <c r="B210" s="109"/>
       <c r="C210" s="109"/>
@@ -51194,7 +51972,7 @@
     </row>
     <row r="211" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A211" s="13" t="s">
-        <v>843</v>
+        <v>905</v>
       </c>
       <c r="B211" s="13"/>
       <c r="C211" s="13"/>
@@ -51243,7 +52021,7 @@
       <c r="AL211" s="93"/>
       <c r="AM211" s="93"/>
       <c r="AN211" s="93" t="s">
-        <v>844</v>
+        <v>906</v>
       </c>
       <c r="AO211" s="93"/>
       <c r="AP211" s="93"/>
@@ -51303,7 +52081,7 @@
     </row>
     <row r="212" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="109" t="s">
-        <v>845</v>
+        <v>907</v>
       </c>
       <c r="B212" s="109"/>
       <c r="C212" s="109"/>
@@ -51562,7 +52340,7 @@
     </row>
     <row r="213" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A213" s="13" t="s">
-        <v>846</v>
+        <v>908</v>
       </c>
       <c r="B213" s="13"/>
       <c r="C213" s="13"/>
@@ -51611,7 +52389,7 @@
       <c r="AL213" s="93"/>
       <c r="AM213" s="93"/>
       <c r="AN213" s="93" t="s">
-        <v>847</v>
+        <v>909</v>
       </c>
       <c r="AO213" s="93"/>
       <c r="AP213" s="93"/>
@@ -51671,7 +52449,7 @@
     </row>
     <row r="214" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A214" s="80" t="s">
-        <v>848</v>
+        <v>910</v>
       </c>
       <c r="B214" s="80"/>
       <c r="C214" s="80"/>
@@ -51930,7 +52708,7 @@
     </row>
     <row r="215" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A215" s="91" t="s">
-        <v>849</v>
+        <v>911</v>
       </c>
       <c r="B215" s="91"/>
       <c r="C215" s="91"/>
@@ -51979,7 +52757,7 @@
       <c r="AL215" s="93"/>
       <c r="AM215" s="93"/>
       <c r="AN215" s="93" t="s">
-        <v>850</v>
+        <v>912</v>
       </c>
       <c r="AO215" s="93"/>
       <c r="AP215" s="93"/>
@@ -52020,14 +52798,14 @@
       <c r="BY215" s="93"/>
       <c r="BZ215" s="93"/>
       <c r="CA215" s="93"/>
-      <c r="CB215" s="187" t="s">
+      <c r="CB215" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC215" s="187"/>
-      <c r="CD215" s="187"/>
-      <c r="CE215" s="187"/>
-      <c r="CF215" s="187"/>
-      <c r="CG215" s="187"/>
+      <c r="CC215" s="202"/>
+      <c r="CD215" s="202"/>
+      <c r="CE215" s="202"/>
+      <c r="CF215" s="202"/>
+      <c r="CG215" s="202"/>
       <c r="CH215" s="93" t="str">
         <f aca="false">IF(CH216=0,"-", "+")</f>
         <v>+</v>
@@ -52039,7 +52817,7 @@
     </row>
     <row r="216" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="80" t="s">
-        <v>851</v>
+        <v>913</v>
       </c>
       <c r="B216" s="80"/>
       <c r="C216" s="80"/>
@@ -52298,7 +53076,7 @@
     </row>
     <row r="217" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="91" t="s">
-        <v>852</v>
+        <v>914</v>
       </c>
       <c r="B217" s="91"/>
       <c r="C217" s="91"/>
@@ -52347,7 +53125,7 @@
       <c r="AL217" s="93"/>
       <c r="AM217" s="93"/>
       <c r="AN217" s="93" t="s">
-        <v>853</v>
+        <v>915</v>
       </c>
       <c r="AO217" s="93"/>
       <c r="AP217" s="93"/>
@@ -52388,14 +53166,14 @@
       <c r="BY217" s="93"/>
       <c r="BZ217" s="93"/>
       <c r="CA217" s="93"/>
-      <c r="CB217" s="187" t="s">
+      <c r="CB217" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC217" s="187"/>
-      <c r="CD217" s="187"/>
-      <c r="CE217" s="187"/>
-      <c r="CF217" s="187"/>
-      <c r="CG217" s="187"/>
+      <c r="CC217" s="202"/>
+      <c r="CD217" s="202"/>
+      <c r="CE217" s="202"/>
+      <c r="CF217" s="202"/>
+      <c r="CG217" s="202"/>
       <c r="CH217" s="93" t="str">
         <f aca="false">IF(CH218=0,"-", "+")</f>
         <v>+</v>
@@ -52407,7 +53185,7 @@
     </row>
     <row r="218" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A218" s="80" t="s">
-        <v>854</v>
+        <v>916</v>
       </c>
       <c r="B218" s="80"/>
       <c r="C218" s="80"/>
@@ -52665,11 +53443,11 @@
       </c>
     </row>
     <row r="219" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A219" s="188" t="s">
-        <v>855</v>
-      </c>
-      <c r="B219" s="188"/>
-      <c r="C219" s="188"/>
+      <c r="A219" s="207" t="s">
+        <v>917</v>
+      </c>
+      <c r="B219" s="207"/>
+      <c r="C219" s="207"/>
       <c r="D219" s="92" t="s">
         <v>150</v>
       </c>
@@ -52756,14 +53534,14 @@
       <c r="BY219" s="93"/>
       <c r="BZ219" s="93"/>
       <c r="CA219" s="93"/>
-      <c r="CB219" s="187" t="s">
+      <c r="CB219" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC219" s="187"/>
-      <c r="CD219" s="187"/>
-      <c r="CE219" s="187"/>
-      <c r="CF219" s="187"/>
-      <c r="CG219" s="187"/>
+      <c r="CC219" s="202"/>
+      <c r="CD219" s="202"/>
+      <c r="CE219" s="202"/>
+      <c r="CF219" s="202"/>
+      <c r="CG219" s="202"/>
       <c r="CH219" s="93" t="str">
         <f aca="false">IF(CH220=0,"-", "+")</f>
         <v>+</v>
@@ -52775,7 +53553,7 @@
     </row>
     <row r="220" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A220" s="109" t="s">
-        <v>856</v>
+        <v>918</v>
       </c>
       <c r="B220" s="109"/>
       <c r="C220" s="109"/>
@@ -53034,12 +53812,12 @@
     </row>
     <row r="221" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A221" s="13" t="s">
-        <v>857</v>
+        <v>919</v>
       </c>
       <c r="B221" s="13"/>
       <c r="C221" s="13"/>
       <c r="D221" s="92" t="s">
-        <v>858</v>
+        <v>920</v>
       </c>
       <c r="E221" s="92"/>
       <c r="F221" s="92"/>
@@ -53083,7 +53861,7 @@
       <c r="AL221" s="93"/>
       <c r="AM221" s="93"/>
       <c r="AN221" s="93" t="s">
-        <v>859</v>
+        <v>921</v>
       </c>
       <c r="AO221" s="93"/>
       <c r="AP221" s="93"/>
@@ -53143,7 +53921,7 @@
     </row>
     <row r="222" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A222" s="80" t="s">
-        <v>860</v>
+        <v>922</v>
       </c>
       <c r="B222" s="80"/>
       <c r="C222" s="80"/>
@@ -53401,11 +54179,11 @@
       </c>
     </row>
     <row r="223" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A223" s="188" t="s">
-        <v>861</v>
-      </c>
-      <c r="B223" s="188"/>
-      <c r="C223" s="188"/>
+      <c r="A223" s="207" t="s">
+        <v>923</v>
+      </c>
+      <c r="B223" s="207"/>
+      <c r="C223" s="207"/>
       <c r="D223" s="92" t="s">
         <v>150</v>
       </c>
@@ -53492,14 +54270,14 @@
       <c r="BY223" s="93"/>
       <c r="BZ223" s="93"/>
       <c r="CA223" s="93"/>
-      <c r="CB223" s="187" t="s">
+      <c r="CB223" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC223" s="187"/>
-      <c r="CD223" s="187"/>
-      <c r="CE223" s="187"/>
-      <c r="CF223" s="187"/>
-      <c r="CG223" s="187"/>
+      <c r="CC223" s="202"/>
+      <c r="CD223" s="202"/>
+      <c r="CE223" s="202"/>
+      <c r="CF223" s="202"/>
+      <c r="CG223" s="202"/>
       <c r="CH223" s="93" t="str">
         <f aca="false">IF(CH224=0,"-", "+")</f>
         <v>+</v>
@@ -53511,7 +54289,7 @@
     </row>
     <row r="224" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A224" s="109" t="s">
-        <v>862</v>
+        <v>924</v>
       </c>
       <c r="B224" s="109"/>
       <c r="C224" s="109"/>
@@ -53770,12 +54548,12 @@
     </row>
     <row r="225" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="13" t="s">
-        <v>863</v>
+        <v>925</v>
       </c>
       <c r="B225" s="13"/>
       <c r="C225" s="13"/>
       <c r="D225" s="92" t="s">
-        <v>864</v>
+        <v>926</v>
       </c>
       <c r="E225" s="92"/>
       <c r="F225" s="92"/>
@@ -53819,7 +54597,7 @@
       <c r="AL225" s="93"/>
       <c r="AM225" s="93"/>
       <c r="AN225" s="93" t="s">
-        <v>865</v>
+        <v>927</v>
       </c>
       <c r="AO225" s="93"/>
       <c r="AP225" s="93"/>
@@ -53879,7 +54657,7 @@
     </row>
     <row r="226" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="80" t="s">
-        <v>866</v>
+        <v>928</v>
       </c>
       <c r="B226" s="80"/>
       <c r="C226" s="80"/>
@@ -54137,11 +54915,11 @@
       </c>
     </row>
     <row r="227" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A227" s="188" t="s">
-        <v>867</v>
-      </c>
-      <c r="B227" s="188"/>
-      <c r="C227" s="188"/>
+      <c r="A227" s="207" t="s">
+        <v>929</v>
+      </c>
+      <c r="B227" s="207"/>
+      <c r="C227" s="207"/>
       <c r="D227" s="92" t="s">
         <v>150</v>
       </c>
@@ -54187,7 +54965,7 @@
       <c r="AL227" s="93"/>
       <c r="AM227" s="93"/>
       <c r="AN227" s="93" t="s">
-        <v>868</v>
+        <v>930</v>
       </c>
       <c r="AO227" s="93"/>
       <c r="AP227" s="93"/>
@@ -54228,14 +55006,14 @@
       <c r="BY227" s="93"/>
       <c r="BZ227" s="93"/>
       <c r="CA227" s="93"/>
-      <c r="CB227" s="187" t="s">
+      <c r="CB227" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC227" s="187"/>
-      <c r="CD227" s="187"/>
-      <c r="CE227" s="187"/>
-      <c r="CF227" s="187"/>
-      <c r="CG227" s="187"/>
+      <c r="CC227" s="202"/>
+      <c r="CD227" s="202"/>
+      <c r="CE227" s="202"/>
+      <c r="CF227" s="202"/>
+      <c r="CG227" s="202"/>
       <c r="CH227" s="93" t="str">
         <f aca="false">IF(CH228=0,"-", "+")</f>
         <v>-</v>
@@ -54247,7 +55025,7 @@
     </row>
     <row r="228" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A228" s="109" t="s">
-        <v>869</v>
+        <v>931</v>
       </c>
       <c r="B228" s="109"/>
       <c r="C228" s="109"/>
@@ -54506,7 +55284,7 @@
     </row>
     <row r="229" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="13" t="s">
-        <v>870</v>
+        <v>932</v>
       </c>
       <c r="B229" s="13"/>
       <c r="C229" s="13"/>
@@ -54615,7 +55393,7 @@
     </row>
     <row r="230" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="109" t="s">
-        <v>871</v>
+        <v>933</v>
       </c>
       <c r="B230" s="109"/>
       <c r="C230" s="109"/>
@@ -54874,12 +55652,12 @@
     </row>
     <row r="231" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="13" t="s">
-        <v>872</v>
+        <v>934</v>
       </c>
       <c r="B231" s="13"/>
       <c r="C231" s="13"/>
       <c r="D231" s="92" t="s">
-        <v>873</v>
+        <v>935</v>
       </c>
       <c r="E231" s="92"/>
       <c r="F231" s="92"/>
@@ -54923,7 +55701,7 @@
       <c r="AL231" s="93"/>
       <c r="AM231" s="93"/>
       <c r="AN231" s="93" t="s">
-        <v>874</v>
+        <v>936</v>
       </c>
       <c r="AO231" s="93"/>
       <c r="AP231" s="93"/>
@@ -54983,7 +55761,7 @@
     </row>
     <row r="232" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="80" t="s">
-        <v>875</v>
+        <v>937</v>
       </c>
       <c r="B232" s="80"/>
       <c r="C232" s="80"/>
@@ -55241,11 +56019,11 @@
       </c>
     </row>
     <row r="233" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A233" s="188" t="s">
-        <v>876</v>
-      </c>
-      <c r="B233" s="188"/>
-      <c r="C233" s="188"/>
+      <c r="A233" s="207" t="s">
+        <v>938</v>
+      </c>
+      <c r="B233" s="207"/>
+      <c r="C233" s="207"/>
       <c r="D233" s="92" t="s">
         <v>150</v>
       </c>
@@ -55291,7 +56069,7 @@
       <c r="AL233" s="93"/>
       <c r="AM233" s="93"/>
       <c r="AN233" s="93" t="s">
-        <v>877</v>
+        <v>939</v>
       </c>
       <c r="AO233" s="93"/>
       <c r="AP233" s="93"/>
@@ -55332,14 +56110,14 @@
       <c r="BY233" s="93"/>
       <c r="BZ233" s="93"/>
       <c r="CA233" s="93"/>
-      <c r="CB233" s="187" t="s">
+      <c r="CB233" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC233" s="187"/>
-      <c r="CD233" s="187"/>
-      <c r="CE233" s="187"/>
-      <c r="CF233" s="187"/>
-      <c r="CG233" s="187"/>
+      <c r="CC233" s="202"/>
+      <c r="CD233" s="202"/>
+      <c r="CE233" s="202"/>
+      <c r="CF233" s="202"/>
+      <c r="CG233" s="202"/>
       <c r="CH233" s="93" t="str">
         <f aca="false">IF(CH234=0,"-", "+")</f>
         <v>-</v>
@@ -55351,7 +56129,7 @@
     </row>
     <row r="234" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A234" s="109" t="s">
-        <v>878</v>
+        <v>940</v>
       </c>
       <c r="B234" s="109"/>
       <c r="C234" s="109"/>
@@ -55610,7 +56388,7 @@
     </row>
     <row r="235" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="13" t="s">
-        <v>879</v>
+        <v>941</v>
       </c>
       <c r="B235" s="13"/>
       <c r="C235" s="13"/>
@@ -55719,7 +56497,7 @@
     </row>
     <row r="236" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A236" s="109" t="s">
-        <v>880</v>
+        <v>942</v>
       </c>
       <c r="B236" s="109"/>
       <c r="C236" s="109"/>
@@ -55978,12 +56756,12 @@
     </row>
     <row r="237" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="13" t="s">
-        <v>881</v>
+        <v>943</v>
       </c>
       <c r="B237" s="13"/>
       <c r="C237" s="13"/>
       <c r="D237" s="92" t="s">
-        <v>873</v>
+        <v>935</v>
       </c>
       <c r="E237" s="92"/>
       <c r="F237" s="92"/>
@@ -56027,7 +56805,7 @@
       <c r="AL237" s="93"/>
       <c r="AM237" s="93"/>
       <c r="AN237" s="93" t="s">
-        <v>874</v>
+        <v>936</v>
       </c>
       <c r="AO237" s="93"/>
       <c r="AP237" s="93"/>
@@ -56087,7 +56865,7 @@
     </row>
     <row r="238" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="80" t="s">
-        <v>882</v>
+        <v>944</v>
       </c>
       <c r="B238" s="80"/>
       <c r="C238" s="80"/>
@@ -56345,11 +57123,11 @@
       </c>
     </row>
     <row r="239" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A239" s="188" t="s">
-        <v>883</v>
-      </c>
-      <c r="B239" s="188"/>
-      <c r="C239" s="188"/>
+      <c r="A239" s="207" t="s">
+        <v>945</v>
+      </c>
+      <c r="B239" s="207"/>
+      <c r="C239" s="207"/>
       <c r="D239" s="92" t="s">
         <v>166</v>
       </c>
@@ -56395,7 +57173,7 @@
       <c r="AL239" s="93"/>
       <c r="AM239" s="93"/>
       <c r="AN239" s="93" t="s">
-        <v>884</v>
+        <v>946</v>
       </c>
       <c r="AO239" s="93"/>
       <c r="AP239" s="93"/>
@@ -56436,14 +57214,14 @@
       <c r="BY239" s="93"/>
       <c r="BZ239" s="93"/>
       <c r="CA239" s="93"/>
-      <c r="CB239" s="187" t="s">
+      <c r="CB239" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC239" s="187"/>
-      <c r="CD239" s="187"/>
-      <c r="CE239" s="187"/>
-      <c r="CF239" s="187"/>
-      <c r="CG239" s="187"/>
+      <c r="CC239" s="202"/>
+      <c r="CD239" s="202"/>
+      <c r="CE239" s="202"/>
+      <c r="CF239" s="202"/>
+      <c r="CG239" s="202"/>
       <c r="CH239" s="93" t="str">
         <f aca="false">IF(CH240=0,"-", "+")</f>
         <v>+</v>
@@ -56455,7 +57233,7 @@
     </row>
     <row r="240" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="80" t="s">
-        <v>885</v>
+        <v>947</v>
       </c>
       <c r="B240" s="80"/>
       <c r="C240" s="80"/>
@@ -56714,7 +57492,7 @@
     </row>
     <row r="241" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="91" t="s">
-        <v>886</v>
+        <v>948</v>
       </c>
       <c r="B241" s="91"/>
       <c r="C241" s="91"/>
@@ -56804,14 +57582,14 @@
       <c r="BY241" s="93"/>
       <c r="BZ241" s="93"/>
       <c r="CA241" s="93"/>
-      <c r="CB241" s="187" t="s">
+      <c r="CB241" s="202" t="s">
         <v>155</v>
       </c>
-      <c r="CC241" s="187"/>
-      <c r="CD241" s="187"/>
-      <c r="CE241" s="187"/>
-      <c r="CF241" s="187"/>
-      <c r="CG241" s="187"/>
+      <c r="CC241" s="202"/>
+      <c r="CD241" s="202"/>
+      <c r="CE241" s="202"/>
+      <c r="CF241" s="202"/>
+      <c r="CG241" s="202"/>
       <c r="CH241" s="93" t="str">
         <f aca="false">IF(CH242=0,"-", "+")</f>
         <v>+</v>
@@ -56823,7 +57601,7 @@
     </row>
     <row r="242" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A242" s="80" t="s">
-        <v>887</v>
+        <v>949</v>
       </c>
       <c r="B242" s="80"/>
       <c r="C242" s="80"/>
@@ -57081,11 +57859,11 @@
       </c>
     </row>
     <row r="243" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A243" s="188" t="s">
-        <v>888</v>
-      </c>
-      <c r="B243" s="188"/>
-      <c r="C243" s="188"/>
+      <c r="A243" s="207" t="s">
+        <v>950</v>
+      </c>
+      <c r="B243" s="207"/>
+      <c r="C243" s="207"/>
       <c r="D243" s="92" t="s">
         <v>166</v>
       </c>
@@ -57131,7 +57909,7 @@
       <c r="AL243" s="93"/>
       <c r="AM243" s="93"/>
       <c r="AN243" s="93" t="s">
-        <v>889</v>
+        <v>951</v>
       </c>
       <c r="AO243" s="93"/>
       <c r="AP243" s="93"/>
@@ -57172,14 +57950,14 @@
       <c r="BY243" s="93"/>
       <c r="BZ243" s="93"/>
       <c r="CA243" s="93"/>
-      <c r="CB243" s="187" t="s">
-        <v>890</v>
-      </c>
-      <c r="CC243" s="187"/>
-      <c r="CD243" s="187"/>
-      <c r="CE243" s="187"/>
-      <c r="CF243" s="187"/>
-      <c r="CG243" s="187"/>
+      <c r="CB243" s="202" t="s">
+        <v>952</v>
+      </c>
+      <c r="CC243" s="202"/>
+      <c r="CD243" s="202"/>
+      <c r="CE243" s="202"/>
+      <c r="CF243" s="202"/>
+      <c r="CG243" s="202"/>
       <c r="CH243" s="93" t="str">
         <f aca="false">IF(CH244=0,"-", "+")</f>
         <v>+</v>
@@ -57191,7 +57969,7 @@
     </row>
     <row r="244" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A244" s="80" t="s">
-        <v>891</v>
+        <v>953</v>
       </c>
       <c r="B244" s="80"/>
       <c r="C244" s="80"/>
@@ -57449,13 +58227,13 @@
       </c>
     </row>
     <row r="245" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A245" s="188" t="s">
-        <v>892</v>
-      </c>
-      <c r="B245" s="188"/>
-      <c r="C245" s="188"/>
+      <c r="A245" s="207" t="s">
+        <v>954</v>
+      </c>
+      <c r="B245" s="207"/>
+      <c r="C245" s="207"/>
       <c r="D245" s="92" t="s">
-        <v>893</v>
+        <v>955</v>
       </c>
       <c r="E245" s="92"/>
       <c r="F245" s="92"/>
@@ -57499,7 +58277,7 @@
       <c r="AL245" s="93"/>
       <c r="AM245" s="93"/>
       <c r="AN245" s="93" t="s">
-        <v>889</v>
+        <v>951</v>
       </c>
       <c r="AO245" s="93"/>
       <c r="AP245" s="93"/>
@@ -57540,14 +58318,14 @@
       <c r="BY245" s="93"/>
       <c r="BZ245" s="93"/>
       <c r="CA245" s="93"/>
-      <c r="CB245" s="187" t="s">
-        <v>890</v>
-      </c>
-      <c r="CC245" s="187"/>
-      <c r="CD245" s="187"/>
-      <c r="CE245" s="187"/>
-      <c r="CF245" s="187"/>
-      <c r="CG245" s="187"/>
+      <c r="CB245" s="202" t="s">
+        <v>952</v>
+      </c>
+      <c r="CC245" s="202"/>
+      <c r="CD245" s="202"/>
+      <c r="CE245" s="202"/>
+      <c r="CF245" s="202"/>
+      <c r="CG245" s="202"/>
       <c r="CH245" s="93" t="str">
         <f aca="false">IF(CH246=0,"-", "+")</f>
         <v>+</v>
@@ -57559,7 +58337,7 @@
     </row>
     <row r="246" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="80" t="s">
-        <v>894</v>
+        <v>956</v>
       </c>
       <c r="B246" s="80"/>
       <c r="C246" s="80"/>
@@ -57817,7 +58595,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1967">
+  <mergeCells count="2013">
     <mergeCell ref="A1:C3"/>
     <mergeCell ref="CK1:CL1"/>
     <mergeCell ref="CM1:CO1"/>
@@ -59280,7 +60058,17 @@
     <mergeCell ref="AH119:AM119"/>
     <mergeCell ref="AN119:CA119"/>
     <mergeCell ref="CB119:CG119"/>
+    <mergeCell ref="CQ119:CS120"/>
+    <mergeCell ref="CT119:CV119"/>
+    <mergeCell ref="CW119:DI119"/>
+    <mergeCell ref="DJ119:EC119"/>
     <mergeCell ref="A120:C120"/>
+    <mergeCell ref="DR120:DS120"/>
+    <mergeCell ref="DT120:DU120"/>
+    <mergeCell ref="DV120:DW120"/>
+    <mergeCell ref="DX120:DY120"/>
+    <mergeCell ref="DZ120:EA120"/>
+    <mergeCell ref="EB120:EC120"/>
     <mergeCell ref="A121:C121"/>
     <mergeCell ref="D121:H121"/>
     <mergeCell ref="I121:N121"/>
@@ -59288,7 +60076,9 @@
     <mergeCell ref="AH121:AM121"/>
     <mergeCell ref="AN121:CA121"/>
     <mergeCell ref="CB121:CG121"/>
+    <mergeCell ref="CQ121:CS121"/>
     <mergeCell ref="A122:C122"/>
+    <mergeCell ref="CQ122:CS122"/>
     <mergeCell ref="A123:C123"/>
     <mergeCell ref="D123:H123"/>
     <mergeCell ref="I123:N123"/>
@@ -59296,7 +60086,9 @@
     <mergeCell ref="AH123:AM123"/>
     <mergeCell ref="AN123:CA123"/>
     <mergeCell ref="CB123:CG123"/>
+    <mergeCell ref="CQ123:CS123"/>
     <mergeCell ref="A124:C124"/>
+    <mergeCell ref="CQ124:CS124"/>
     <mergeCell ref="A125:C125"/>
     <mergeCell ref="D125:H125"/>
     <mergeCell ref="I125:N125"/>
@@ -59304,7 +60096,9 @@
     <mergeCell ref="AH125:AM125"/>
     <mergeCell ref="AN125:CA125"/>
     <mergeCell ref="CB125:CG125"/>
+    <mergeCell ref="CQ125:CS125"/>
     <mergeCell ref="A126:C126"/>
+    <mergeCell ref="CQ126:CS126"/>
     <mergeCell ref="A127:C127"/>
     <mergeCell ref="D127:H127"/>
     <mergeCell ref="I127:N127"/>
@@ -59312,7 +60106,9 @@
     <mergeCell ref="AH127:AM127"/>
     <mergeCell ref="AN127:CA127"/>
     <mergeCell ref="CB127:CG127"/>
+    <mergeCell ref="CQ127:CS127"/>
     <mergeCell ref="A128:C128"/>
+    <mergeCell ref="CQ128:CS128"/>
     <mergeCell ref="A129:C129"/>
     <mergeCell ref="D129:H129"/>
     <mergeCell ref="I129:N129"/>
@@ -59320,7 +60116,9 @@
     <mergeCell ref="AH129:AM129"/>
     <mergeCell ref="AN129:CA129"/>
     <mergeCell ref="CB129:CG129"/>
+    <mergeCell ref="CQ129:CS129"/>
     <mergeCell ref="A130:C130"/>
+    <mergeCell ref="CQ130:CS130"/>
     <mergeCell ref="A131:C131"/>
     <mergeCell ref="D131:H131"/>
     <mergeCell ref="I131:N131"/>
@@ -59328,7 +60126,9 @@
     <mergeCell ref="AH131:AM131"/>
     <mergeCell ref="AN131:CA131"/>
     <mergeCell ref="CB131:CG131"/>
+    <mergeCell ref="CQ131:CS131"/>
     <mergeCell ref="A132:C132"/>
+    <mergeCell ref="CQ132:CS132"/>
     <mergeCell ref="A133:C133"/>
     <mergeCell ref="D133:H133"/>
     <mergeCell ref="I133:N133"/>
@@ -59336,7 +60136,9 @@
     <mergeCell ref="AH133:AM133"/>
     <mergeCell ref="AN133:CA133"/>
     <mergeCell ref="CB133:CG133"/>
+    <mergeCell ref="CQ133:CS133"/>
     <mergeCell ref="A134:C134"/>
+    <mergeCell ref="CQ134:CS134"/>
     <mergeCell ref="A135:C135"/>
     <mergeCell ref="D135:H135"/>
     <mergeCell ref="I135:N135"/>
@@ -59344,7 +60146,9 @@
     <mergeCell ref="AH135:AM135"/>
     <mergeCell ref="AN135:CA135"/>
     <mergeCell ref="CB135:CG135"/>
+    <mergeCell ref="CQ135:CS135"/>
     <mergeCell ref="A136:C136"/>
+    <mergeCell ref="CQ136:CS136"/>
     <mergeCell ref="A137:C137"/>
     <mergeCell ref="D137:H137"/>
     <mergeCell ref="I137:N137"/>
@@ -59352,7 +60156,9 @@
     <mergeCell ref="AH137:AM137"/>
     <mergeCell ref="AN137:CA137"/>
     <mergeCell ref="CB137:CG137"/>
+    <mergeCell ref="CQ137:CS137"/>
     <mergeCell ref="A138:C138"/>
+    <mergeCell ref="CQ138:CS138"/>
     <mergeCell ref="A139:C139"/>
     <mergeCell ref="D139:H139"/>
     <mergeCell ref="I139:N139"/>
@@ -59360,7 +60166,9 @@
     <mergeCell ref="AH139:AM139"/>
     <mergeCell ref="AN139:CA139"/>
     <mergeCell ref="CB139:CG139"/>
+    <mergeCell ref="CQ139:CS139"/>
     <mergeCell ref="A140:C140"/>
+    <mergeCell ref="CQ140:CS140"/>
     <mergeCell ref="A141:C141"/>
     <mergeCell ref="D141:H141"/>
     <mergeCell ref="I141:N141"/>
@@ -59368,7 +60176,9 @@
     <mergeCell ref="AH141:AM141"/>
     <mergeCell ref="AN141:CA141"/>
     <mergeCell ref="CB141:CG141"/>
+    <mergeCell ref="CQ141:CS141"/>
     <mergeCell ref="A142:C142"/>
+    <mergeCell ref="CQ142:CS142"/>
     <mergeCell ref="A143:C143"/>
     <mergeCell ref="D143:H143"/>
     <mergeCell ref="I143:N143"/>
@@ -59376,7 +60186,9 @@
     <mergeCell ref="AH143:AM143"/>
     <mergeCell ref="AN143:CA143"/>
     <mergeCell ref="CB143:CG143"/>
+    <mergeCell ref="CQ143:CS143"/>
     <mergeCell ref="A144:C144"/>
+    <mergeCell ref="CQ144:CS144"/>
     <mergeCell ref="A145:C145"/>
     <mergeCell ref="D145:H145"/>
     <mergeCell ref="I145:N145"/>
@@ -59384,7 +60196,9 @@
     <mergeCell ref="AH145:AM145"/>
     <mergeCell ref="AN145:CA145"/>
     <mergeCell ref="CB145:CG145"/>
+    <mergeCell ref="CQ145:CS145"/>
     <mergeCell ref="A146:C146"/>
+    <mergeCell ref="CQ146:CS146"/>
     <mergeCell ref="A147:C147"/>
     <mergeCell ref="D147:H147"/>
     <mergeCell ref="I147:N147"/>
@@ -59392,7 +60206,9 @@
     <mergeCell ref="AH147:AM147"/>
     <mergeCell ref="AN147:CA147"/>
     <mergeCell ref="CB147:CG147"/>
+    <mergeCell ref="CQ147:CS147"/>
     <mergeCell ref="A148:C148"/>
+    <mergeCell ref="CQ148:CS148"/>
     <mergeCell ref="A149:C149"/>
     <mergeCell ref="D149:H149"/>
     <mergeCell ref="I149:N149"/>
@@ -59400,7 +60216,9 @@
     <mergeCell ref="AH149:AM149"/>
     <mergeCell ref="AN149:CA149"/>
     <mergeCell ref="CB149:CG149"/>
+    <mergeCell ref="CQ149:CS149"/>
     <mergeCell ref="A150:C150"/>
+    <mergeCell ref="CQ150:CS150"/>
     <mergeCell ref="A151:C151"/>
     <mergeCell ref="D151:H151"/>
     <mergeCell ref="I151:N151"/>
@@ -59408,7 +60226,9 @@
     <mergeCell ref="AH151:AM151"/>
     <mergeCell ref="AN151:CA151"/>
     <mergeCell ref="CB151:CG151"/>
+    <mergeCell ref="CQ151:CS151"/>
     <mergeCell ref="A152:C152"/>
+    <mergeCell ref="CQ152:CS152"/>
     <mergeCell ref="A153:C153"/>
     <mergeCell ref="D153:H153"/>
     <mergeCell ref="I153:N153"/>
@@ -59416,7 +60236,9 @@
     <mergeCell ref="AH153:AM153"/>
     <mergeCell ref="AN153:CA153"/>
     <mergeCell ref="CB153:CG153"/>
+    <mergeCell ref="CQ153:CS153"/>
     <mergeCell ref="A154:C154"/>
+    <mergeCell ref="CQ154:CS154"/>
     <mergeCell ref="A155:C155"/>
     <mergeCell ref="D155:H155"/>
     <mergeCell ref="I155:N155"/>
@@ -59424,7 +60246,9 @@
     <mergeCell ref="AH155:AM155"/>
     <mergeCell ref="AN155:CA155"/>
     <mergeCell ref="CB155:CG155"/>
+    <mergeCell ref="CQ155:CS155"/>
     <mergeCell ref="A156:C156"/>
+    <mergeCell ref="CQ156:CS156"/>
     <mergeCell ref="A157:C157"/>
     <mergeCell ref="D157:H157"/>
     <mergeCell ref="I157:N157"/>

</xml_diff>

<commit_message>
Added one new token (NameLiteralWithIndexToken) and minor code updates TEXT_Instruction is still WiP, better ways are soon to be found
</commit_message>
<xml_diff>
--- a/16-Bit Computer Manual v2.xlsx
+++ b/16-Bit Computer Manual v2.xlsx
@@ -5080,9 +5080,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <dxfs count="1">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-    </dxf>
+    <dxf/>
   </dxfs>
   <colors>
     <indexedColors>
@@ -5154,8 +5152,8 @@
   </sheetPr>
   <dimension ref="A1:EL246"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AC1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BP4" activeCellId="1" sqref="CB1:CG1 BP4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Next run is soon to begin Merged AccessLabelToken with and without Indices, same for NameLiteralToken
</commit_message>
<xml_diff>
--- a/16-Bit Computer Manual v2.xlsx
+++ b/16-Bit Computer Manual v2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2021" uniqueCount="957">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2024" uniqueCount="960">
   <si>
     <t xml:space="preserve">ADDRESS</t>
   </si>
@@ -2719,190 +2719,199 @@
     <t xml:space="preserve">RET I </t>
   </si>
   <si>
+    <t xml:space="preserve">NameLiteralWithIndex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x003C</t>
+  </si>
+  <si>
     <t xml:space="preserve">Operator</t>
   </si>
   <si>
-    <t xml:space="preserve">0x003C</t>
+    <t xml:space="preserve">RET II</t>
   </si>
   <si>
     <t xml:space="preserve">RegistryAccess</t>
   </si>
   <si>
-    <t xml:space="preserve">RET II</t>
+    <t xml:space="preserve">0x003D</t>
   </si>
   <si>
     <t xml:space="preserve">StringLiteral</t>
   </si>
   <si>
-    <t xml:space="preserve">0x003D</t>
+    <t xml:space="preserve">RET III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DBUS -&gt; PC</t>
   </si>
   <si>
     <t xml:space="preserve">AccLab | AccLab</t>
   </si>
   <si>
-    <t xml:space="preserve">RET III</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DBUS -&gt; PC</t>
+    <t xml:space="preserve">0x003E</t>
   </si>
   <si>
     <t xml:space="preserve">AccLab | ALWIndex</t>
   </si>
   <si>
-    <t xml:space="preserve">0x003E</t>
+    <t xml:space="preserve">RET IV</t>
   </si>
   <si>
     <t xml:space="preserve">AccLab | Array</t>
   </si>
   <si>
-    <t xml:space="preserve">RET IV</t>
+    <t xml:space="preserve">0x003F</t>
   </si>
   <si>
     <t xml:space="preserve">AccLab | EntryL</t>
   </si>
   <si>
-    <t xml:space="preserve">0x003F</t>
+    <t xml:space="preserve">PRINT RB I </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RB := RB + 0 (for translating the result over ALU)</t>
   </si>
   <si>
     <t xml:space="preserve">AccLab | IntExp</t>
   </si>
   <si>
-    <t xml:space="preserve">PRINT RB I </t>
-  </si>
-  <si>
-    <t xml:space="preserve">RB := RB + 0 (for translating the result over ALU)</t>
+    <t xml:space="preserve">0x0040</t>
   </si>
   <si>
     <t xml:space="preserve">AccLab | JmpL</t>
   </si>
   <si>
-    <t xml:space="preserve">0x0040</t>
+    <t xml:space="preserve">MOV ESP, EBP I </t>
   </si>
   <si>
     <t xml:space="preserve">AccLab | NameL</t>
   </si>
   <si>
-    <t xml:space="preserve">MOV ESP, EBP I </t>
+    <t xml:space="preserve">0x0041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AccLab | NLWIndex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV ESP, EBP II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rB15 -&gt; DBUS</t>
   </si>
   <si>
     <t xml:space="preserve">AccLab | OP</t>
   </si>
   <si>
-    <t xml:space="preserve">0x0041</t>
+    <t xml:space="preserve">0x0042</t>
   </si>
   <si>
     <t xml:space="preserve">AccLab | RegAcc</t>
   </si>
   <si>
-    <t xml:space="preserve">MOV ESP, EBP II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rB15 -&gt; DBUS</t>
+    <t xml:space="preserve">MOV EBP, ESP I </t>
   </si>
   <si>
     <t xml:space="preserve">AccLab | StringL</t>
   </si>
   <si>
-    <t xml:space="preserve">0x0042</t>
+    <t xml:space="preserve">0x0043</t>
   </si>
   <si>
     <t xml:space="preserve">ALWIndex | AccLab</t>
   </si>
   <si>
-    <t xml:space="preserve">MOV EBP, ESP I </t>
+    <t xml:space="preserve">MOV EBP, ESP II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DBUS -&gt; EBP</t>
   </si>
   <si>
     <t xml:space="preserve">ALWIndex | ALWIndex</t>
   </si>
   <si>
-    <t xml:space="preserve">0x0043</t>
+    <t xml:space="preserve">0x0044</t>
   </si>
   <si>
     <t xml:space="preserve">ALWIndex | Array</t>
   </si>
   <si>
-    <t xml:space="preserve">MOV EBP, ESP II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DBUS -&gt; EBP</t>
+    <t xml:space="preserve">PUSH EBP I </t>
   </si>
   <si>
     <t xml:space="preserve">ALWIndex | EntryL</t>
   </si>
   <si>
-    <t xml:space="preserve">0x0044</t>
+    <t xml:space="preserve">0x0045</t>
   </si>
   <si>
     <t xml:space="preserve">ALWIndex | IntExp</t>
   </si>
   <si>
-    <t xml:space="preserve">PUSH EBP I </t>
+    <t xml:space="preserve">PUSH EBP II</t>
   </si>
   <si>
     <t xml:space="preserve">ALWIndex | JmpL</t>
   </si>
   <si>
-    <t xml:space="preserve">0x0045</t>
+    <t xml:space="preserve">0x0046</t>
   </si>
   <si>
     <t xml:space="preserve">ALWIndex | NameL</t>
   </si>
   <si>
-    <t xml:space="preserve">PUSH EBP II</t>
+    <t xml:space="preserve">PUSH EBP III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALWIndex | NLWIndex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0047</t>
   </si>
   <si>
     <t xml:space="preserve">ALWIndex | OP</t>
   </si>
   <si>
-    <t xml:space="preserve">0x0046</t>
+    <t xml:space="preserve">PUSH EBP IV</t>
   </si>
   <si>
     <t xml:space="preserve">ALWIndex | RegAcc</t>
   </si>
   <si>
-    <t xml:space="preserve">PUSH EBP III</t>
+    <t xml:space="preserve">0x0048</t>
   </si>
   <si>
     <t xml:space="preserve">ALWIndex | StringL</t>
   </si>
   <si>
-    <t xml:space="preserve">0x0047</t>
+    <t xml:space="preserve">POP EBP I </t>
   </si>
   <si>
     <t xml:space="preserve">Array | AccLab</t>
   </si>
   <si>
-    <t xml:space="preserve">PUSH EBP IV</t>
+    <t xml:space="preserve">0x0049</t>
   </si>
   <si>
     <t xml:space="preserve">Array | ALWIndex</t>
   </si>
   <si>
-    <t xml:space="preserve">0x0048</t>
+    <t xml:space="preserve">POP EBP II</t>
   </si>
   <si>
     <t xml:space="preserve">Array | Array</t>
   </si>
   <si>
-    <t xml:space="preserve">POP EBP I </t>
+    <t xml:space="preserve">0x004A</t>
   </si>
   <si>
     <t xml:space="preserve">Array | EntryL</t>
   </si>
   <si>
-    <t xml:space="preserve">0x0049</t>
+    <t xml:space="preserve">POP EBP III</t>
   </si>
   <si>
     <t xml:space="preserve">Array | IntExp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POP EBP II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x004A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POP EBP III</t>
   </si>
   <si>
     <t xml:space="preserve">0x004B</t>
@@ -5152,8 +5161,8 @@
   </sheetPr>
   <dimension ref="A1:EL246"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AC1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BP4" activeCellId="1" sqref="CB1:CG1 BP4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CK128" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CQ152" activeCellId="0" sqref="CQ152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -37199,14 +37208,14 @@
         <f aca="false">IF(CI132=0,"-", "+")</f>
         <v>-</v>
       </c>
-      <c r="CQ131" s="203" t="s">
+      <c r="CQ131" s="192" t="s">
         <v>780</v>
       </c>
-      <c r="CR131" s="203"/>
-      <c r="CS131" s="203"/>
-      <c r="CT131" s="204"/>
-      <c r="CU131" s="205"/>
-      <c r="CV131" s="206"/>
+      <c r="CR131" s="192"/>
+      <c r="CS131" s="192"/>
+      <c r="CT131" s="199"/>
+      <c r="CU131" s="200"/>
+      <c r="CV131" s="201"/>
     </row>
     <row r="132" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="109" t="s">
@@ -37466,11 +37475,14 @@
       <c r="CI132" s="51" t="n">
         <v>0</v>
       </c>
-      <c r="CQ132" s="192" t="s">
+      <c r="CQ132" s="203" t="s">
         <v>782</v>
       </c>
-      <c r="CR132" s="192"/>
-      <c r="CS132" s="192"/>
+      <c r="CR132" s="203"/>
+      <c r="CS132" s="203"/>
+      <c r="CT132" s="204"/>
+      <c r="CU132" s="205"/>
+      <c r="CV132" s="206"/>
     </row>
     <row r="133" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="186" t="s">
@@ -38983,6 +38995,9 @@
       </c>
       <c r="CR140" s="192"/>
       <c r="CS140" s="192"/>
+      <c r="CT140" s="0"/>
+      <c r="CU140" s="0"/>
+      <c r="CV140" s="0"/>
     </row>
     <row r="141" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="13" t="s">
@@ -39092,14 +39107,11 @@
         <f aca="false">IF(CI142=0,"-", "+")</f>
         <v>-</v>
       </c>
-      <c r="CQ141" s="203" t="s">
+      <c r="CQ141" s="192" t="s">
         <v>803</v>
       </c>
-      <c r="CR141" s="203"/>
-      <c r="CS141" s="203"/>
-      <c r="CT141" s="208"/>
-      <c r="CU141" s="208"/>
-      <c r="CV141" s="208"/>
+      <c r="CR141" s="192"/>
+      <c r="CS141" s="192"/>
     </row>
     <row r="142" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="80" t="s">
@@ -39473,11 +39485,14 @@
         <f aca="false">IF(CI144=0,"-", "+")</f>
         <v>-</v>
       </c>
-      <c r="CQ143" s="192" t="s">
+      <c r="CQ143" s="203" t="s">
         <v>807</v>
       </c>
-      <c r="CR143" s="192"/>
-      <c r="CS143" s="192"/>
+      <c r="CR143" s="203"/>
+      <c r="CS143" s="203"/>
+      <c r="CT143" s="208"/>
+      <c r="CU143" s="208"/>
+      <c r="CV143" s="208"/>
     </row>
     <row r="144" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="109" t="s">
@@ -40985,14 +41000,14 @@
         <f aca="false">IF(CI152=0,"-", "+")</f>
         <v>-</v>
       </c>
-      <c r="CQ151" s="203" t="s">
+      <c r="CQ151" s="192" t="s">
         <v>824</v>
       </c>
-      <c r="CR151" s="203"/>
-      <c r="CS151" s="203"/>
-      <c r="CT151" s="208"/>
-      <c r="CU151" s="208"/>
-      <c r="CV151" s="208"/>
+      <c r="CR151" s="192"/>
+      <c r="CS151" s="192"/>
+      <c r="CT151" s="0"/>
+      <c r="CU151" s="0"/>
+      <c r="CV151" s="0"/>
     </row>
     <row r="152" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="109" t="s">
@@ -41630,11 +41645,14 @@
       <c r="CI154" s="87" t="n">
         <v>0</v>
       </c>
-      <c r="CQ154" s="192" t="s">
+      <c r="CQ154" s="203" t="s">
         <v>830</v>
       </c>
-      <c r="CR154" s="192"/>
-      <c r="CS154" s="192"/>
+      <c r="CR154" s="203"/>
+      <c r="CS154" s="203"/>
+      <c r="CT154" s="208"/>
+      <c r="CU154" s="208"/>
+      <c r="CV154" s="208"/>
     </row>
     <row r="155" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="207" t="s">
@@ -42122,10 +42140,15 @@
         <f aca="false">IF(CI158=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ157" s="192" t="s">
+        <v>836</v>
+      </c>
+      <c r="CR157" s="192"/>
+      <c r="CS157" s="192"/>
     </row>
     <row r="158" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="109" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B158" s="109"/>
       <c r="C158" s="109"/>
@@ -42381,10 +42404,15 @@
       <c r="CI158" s="51" t="n">
         <v>0</v>
       </c>
+      <c r="CQ158" s="192" t="s">
+        <v>838</v>
+      </c>
+      <c r="CR158" s="192"/>
+      <c r="CS158" s="192"/>
     </row>
     <row r="159" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="13" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="B159" s="13"/>
       <c r="C159" s="13"/>
@@ -42490,10 +42518,15 @@
         <f aca="false">IF(CI160=0,"-", "+")</f>
         <v>-</v>
       </c>
+      <c r="CQ159" s="192" t="s">
+        <v>840</v>
+      </c>
+      <c r="CR159" s="192"/>
+      <c r="CS159" s="192"/>
     </row>
     <row r="160" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="109" t="s">
-        <v>838</v>
+        <v>841</v>
       </c>
       <c r="B160" s="109"/>
       <c r="C160" s="109"/>
@@ -42752,7 +42785,7 @@
     </row>
     <row r="161" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="13" t="s">
-        <v>839</v>
+        <v>842</v>
       </c>
       <c r="B161" s="13"/>
       <c r="C161" s="13"/>
@@ -42861,7 +42894,7 @@
     </row>
     <row r="162" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="80" t="s">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="B162" s="80"/>
       <c r="C162" s="80"/>
@@ -43120,7 +43153,7 @@
     </row>
     <row r="163" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="207" t="s">
-        <v>841</v>
+        <v>844</v>
       </c>
       <c r="B163" s="207"/>
       <c r="C163" s="207"/>
@@ -43229,7 +43262,7 @@
     </row>
     <row r="164" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="109" t="s">
-        <v>842</v>
+        <v>845</v>
       </c>
       <c r="B164" s="109"/>
       <c r="C164" s="109"/>
@@ -43488,7 +43521,7 @@
     </row>
     <row r="165" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="13" t="s">
-        <v>843</v>
+        <v>846</v>
       </c>
       <c r="B165" s="13"/>
       <c r="C165" s="13"/>
@@ -43529,7 +43562,7 @@
       <c r="AF165" s="93"/>
       <c r="AG165" s="93"/>
       <c r="AH165" s="93" t="s">
-        <v>844</v>
+        <v>847</v>
       </c>
       <c r="AI165" s="93"/>
       <c r="AJ165" s="93"/>
@@ -43537,7 +43570,7 @@
       <c r="AL165" s="93"/>
       <c r="AM165" s="93"/>
       <c r="AN165" s="93" t="s">
-        <v>845</v>
+        <v>848</v>
       </c>
       <c r="AO165" s="93"/>
       <c r="AP165" s="93"/>
@@ -43597,7 +43630,7 @@
     </row>
     <row r="166" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="109" t="s">
-        <v>846</v>
+        <v>849</v>
       </c>
       <c r="B166" s="109"/>
       <c r="C166" s="109"/>
@@ -43856,7 +43889,7 @@
     </row>
     <row r="167" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="13" t="s">
-        <v>847</v>
+        <v>850</v>
       </c>
       <c r="B167" s="13"/>
       <c r="C167" s="13"/>
@@ -43965,7 +43998,7 @@
     </row>
     <row r="168" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="80" t="s">
-        <v>848</v>
+        <v>851</v>
       </c>
       <c r="B168" s="80"/>
       <c r="C168" s="80"/>
@@ -44224,7 +44257,7 @@
     </row>
     <row r="169" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="207" t="s">
-        <v>849</v>
+        <v>852</v>
       </c>
       <c r="B169" s="207"/>
       <c r="C169" s="207"/>
@@ -44333,7 +44366,7 @@
     </row>
     <row r="170" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="109" t="s">
-        <v>850</v>
+        <v>853</v>
       </c>
       <c r="B170" s="109"/>
       <c r="C170" s="109"/>
@@ -44592,7 +44625,7 @@
     </row>
     <row r="171" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="13" t="s">
-        <v>851</v>
+        <v>854</v>
       </c>
       <c r="B171" s="13"/>
       <c r="C171" s="13"/>
@@ -44633,7 +44666,7 @@
       <c r="AF171" s="93"/>
       <c r="AG171" s="93"/>
       <c r="AH171" s="93" t="s">
-        <v>844</v>
+        <v>847</v>
       </c>
       <c r="AI171" s="93"/>
       <c r="AJ171" s="93"/>
@@ -44641,7 +44674,7 @@
       <c r="AL171" s="93"/>
       <c r="AM171" s="93"/>
       <c r="AN171" s="93" t="s">
-        <v>852</v>
+        <v>855</v>
       </c>
       <c r="AO171" s="93"/>
       <c r="AP171" s="93"/>
@@ -44701,7 +44734,7 @@
     </row>
     <row r="172" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="109" t="s">
-        <v>853</v>
+        <v>856</v>
       </c>
       <c r="B172" s="109"/>
       <c r="C172" s="109"/>
@@ -44960,7 +44993,7 @@
     </row>
     <row r="173" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="13" t="s">
-        <v>854</v>
+        <v>857</v>
       </c>
       <c r="B173" s="13"/>
       <c r="C173" s="13"/>
@@ -45069,7 +45102,7 @@
     </row>
     <row r="174" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="80" t="s">
-        <v>855</v>
+        <v>858</v>
       </c>
       <c r="B174" s="80"/>
       <c r="C174" s="80"/>
@@ -45329,7 +45362,7 @@
     </row>
     <row r="175" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="91" t="s">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c r="B175" s="91"/>
       <c r="C175" s="91"/>
@@ -45349,7 +45382,7 @@
       <c r="M175" s="93"/>
       <c r="N175" s="93"/>
       <c r="O175" s="93" t="s">
-        <v>857</v>
+        <v>860</v>
       </c>
       <c r="P175" s="93"/>
       <c r="Q175" s="93"/>
@@ -45370,7 +45403,7 @@
       <c r="AF175" s="93"/>
       <c r="AG175" s="93"/>
       <c r="AH175" s="93" t="s">
-        <v>858</v>
+        <v>861</v>
       </c>
       <c r="AI175" s="93"/>
       <c r="AJ175" s="93"/>
@@ -45439,7 +45472,7 @@
     </row>
     <row r="176" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="109" t="s">
-        <v>859</v>
+        <v>862</v>
       </c>
       <c r="B176" s="109"/>
       <c r="C176" s="109"/>
@@ -45699,7 +45732,7 @@
     </row>
     <row r="177" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="91" t="s">
-        <v>860</v>
+        <v>863</v>
       </c>
       <c r="B177" s="91"/>
       <c r="C177" s="91"/>
@@ -45816,7 +45849,7 @@
     </row>
     <row r="178" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="109" t="s">
-        <v>861</v>
+        <v>864</v>
       </c>
       <c r="B178" s="109"/>
       <c r="C178" s="109"/>
@@ -46082,7 +46115,7 @@
     </row>
     <row r="179" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="91" t="s">
-        <v>862</v>
+        <v>865</v>
       </c>
       <c r="B179" s="91"/>
       <c r="C179" s="91"/>
@@ -46191,7 +46224,7 @@
     </row>
     <row r="180" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="80" t="s">
-        <v>863</v>
+        <v>866</v>
       </c>
       <c r="B180" s="80"/>
       <c r="C180" s="80"/>
@@ -46450,7 +46483,7 @@
     </row>
     <row r="181" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="91" t="s">
-        <v>864</v>
+        <v>867</v>
       </c>
       <c r="B181" s="91"/>
       <c r="C181" s="91"/>
@@ -46470,7 +46503,7 @@
       <c r="M181" s="93"/>
       <c r="N181" s="93"/>
       <c r="O181" s="93" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="P181" s="93"/>
       <c r="Q181" s="93"/>
@@ -46491,7 +46524,7 @@
       <c r="AF181" s="93"/>
       <c r="AG181" s="93"/>
       <c r="AH181" s="93" t="s">
-        <v>866</v>
+        <v>869</v>
       </c>
       <c r="AI181" s="93"/>
       <c r="AJ181" s="93"/>
@@ -46559,7 +46592,7 @@
     </row>
     <row r="182" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="109" t="s">
-        <v>867</v>
+        <v>870</v>
       </c>
       <c r="B182" s="109"/>
       <c r="C182" s="109"/>
@@ -46818,7 +46851,7 @@
     </row>
     <row r="183" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="91" t="s">
-        <v>868</v>
+        <v>871</v>
       </c>
       <c r="B183" s="91"/>
       <c r="C183" s="91"/>
@@ -46927,7 +46960,7 @@
     </row>
     <row r="184" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="109" t="s">
-        <v>869</v>
+        <v>872</v>
       </c>
       <c r="B184" s="109"/>
       <c r="C184" s="109"/>
@@ -47186,7 +47219,7 @@
     </row>
     <row r="185" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="91" t="s">
-        <v>870</v>
+        <v>873</v>
       </c>
       <c r="B185" s="91"/>
       <c r="C185" s="91"/>
@@ -47295,7 +47328,7 @@
     </row>
     <row r="186" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="80" t="s">
-        <v>871</v>
+        <v>874</v>
       </c>
       <c r="B186" s="80"/>
       <c r="C186" s="80"/>
@@ -47554,7 +47587,7 @@
     </row>
     <row r="187" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="91" t="s">
-        <v>872</v>
+        <v>875</v>
       </c>
       <c r="B187" s="91"/>
       <c r="C187" s="91"/>
@@ -47574,7 +47607,7 @@
       <c r="M187" s="93"/>
       <c r="N187" s="93"/>
       <c r="O187" s="93" t="s">
-        <v>873</v>
+        <v>876</v>
       </c>
       <c r="P187" s="93"/>
       <c r="Q187" s="93"/>
@@ -47595,7 +47628,7 @@
       <c r="AF187" s="93"/>
       <c r="AG187" s="93"/>
       <c r="AH187" s="93" t="s">
-        <v>874</v>
+        <v>877</v>
       </c>
       <c r="AI187" s="93"/>
       <c r="AJ187" s="93"/>
@@ -47663,7 +47696,7 @@
     </row>
     <row r="188" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="109" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
       <c r="B188" s="109"/>
       <c r="C188" s="109"/>
@@ -47922,7 +47955,7 @@
     </row>
     <row r="189" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="91" t="s">
-        <v>876</v>
+        <v>879</v>
       </c>
       <c r="B189" s="91"/>
       <c r="C189" s="91"/>
@@ -48031,7 +48064,7 @@
     </row>
     <row r="190" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="109" t="s">
-        <v>877</v>
+        <v>880</v>
       </c>
       <c r="B190" s="109"/>
       <c r="C190" s="109"/>
@@ -48290,7 +48323,7 @@
     </row>
     <row r="191" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="91" t="s">
-        <v>878</v>
+        <v>881</v>
       </c>
       <c r="B191" s="91"/>
       <c r="C191" s="91"/>
@@ -48399,7 +48432,7 @@
     </row>
     <row r="192" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="80" t="s">
-        <v>879</v>
+        <v>882</v>
       </c>
       <c r="B192" s="80"/>
       <c r="C192" s="80"/>
@@ -48658,7 +48691,7 @@
     </row>
     <row r="193" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="91" t="s">
-        <v>880</v>
+        <v>883</v>
       </c>
       <c r="B193" s="91"/>
       <c r="C193" s="91"/>
@@ -48678,7 +48711,7 @@
       <c r="M193" s="93"/>
       <c r="N193" s="93"/>
       <c r="O193" s="93" t="s">
-        <v>881</v>
+        <v>884</v>
       </c>
       <c r="P193" s="93"/>
       <c r="Q193" s="93"/>
@@ -48699,7 +48732,7 @@
       <c r="AF193" s="93"/>
       <c r="AG193" s="93"/>
       <c r="AH193" s="93" t="s">
-        <v>882</v>
+        <v>885</v>
       </c>
       <c r="AI193" s="93"/>
       <c r="AJ193" s="93"/>
@@ -48767,7 +48800,7 @@
     </row>
     <row r="194" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="109" t="s">
-        <v>883</v>
+        <v>886</v>
       </c>
       <c r="B194" s="109"/>
       <c r="C194" s="109"/>
@@ -49026,7 +49059,7 @@
     </row>
     <row r="195" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="91" t="s">
-        <v>884</v>
+        <v>887</v>
       </c>
       <c r="B195" s="91"/>
       <c r="C195" s="91"/>
@@ -49135,7 +49168,7 @@
     </row>
     <row r="196" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="109" t="s">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c r="B196" s="109"/>
       <c r="C196" s="109"/>
@@ -49394,7 +49427,7 @@
     </row>
     <row r="197" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="91" t="s">
-        <v>886</v>
+        <v>889</v>
       </c>
       <c r="B197" s="91"/>
       <c r="C197" s="91"/>
@@ -49503,7 +49536,7 @@
     </row>
     <row r="198" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="80" t="s">
-        <v>887</v>
+        <v>890</v>
       </c>
       <c r="B198" s="80"/>
       <c r="C198" s="80"/>
@@ -49762,7 +49795,7 @@
     </row>
     <row r="199" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="207" t="s">
-        <v>888</v>
+        <v>891</v>
       </c>
       <c r="B199" s="207"/>
       <c r="C199" s="207"/>
@@ -49811,7 +49844,7 @@
       <c r="AL199" s="93"/>
       <c r="AM199" s="93"/>
       <c r="AN199" s="93" t="s">
-        <v>889</v>
+        <v>892</v>
       </c>
       <c r="AO199" s="93"/>
       <c r="AP199" s="93"/>
@@ -49871,7 +49904,7 @@
     </row>
     <row r="200" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="80" t="s">
-        <v>890</v>
+        <v>893</v>
       </c>
       <c r="B200" s="80"/>
       <c r="C200" s="80"/>
@@ -50130,7 +50163,7 @@
     </row>
     <row r="201" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A201" s="207" t="s">
-        <v>891</v>
+        <v>894</v>
       </c>
       <c r="B201" s="207"/>
       <c r="C201" s="207"/>
@@ -50179,7 +50212,7 @@
       <c r="AL201" s="93"/>
       <c r="AM201" s="93"/>
       <c r="AN201" s="93" t="s">
-        <v>892</v>
+        <v>895</v>
       </c>
       <c r="AO201" s="93"/>
       <c r="AP201" s="93"/>
@@ -50239,7 +50272,7 @@
     </row>
     <row r="202" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="80" t="s">
-        <v>893</v>
+        <v>896</v>
       </c>
       <c r="B202" s="80"/>
       <c r="C202" s="80"/>
@@ -50498,7 +50531,7 @@
     </row>
     <row r="203" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="91" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
       <c r="B203" s="91"/>
       <c r="C203" s="91"/>
@@ -50547,7 +50580,7 @@
       <c r="AL203" s="93"/>
       <c r="AM203" s="93"/>
       <c r="AN203" s="93" t="s">
-        <v>895</v>
+        <v>898</v>
       </c>
       <c r="AO203" s="93"/>
       <c r="AP203" s="93"/>
@@ -50607,7 +50640,7 @@
     </row>
     <row r="204" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="80" t="s">
-        <v>896</v>
+        <v>899</v>
       </c>
       <c r="B204" s="80"/>
       <c r="C204" s="80"/>
@@ -50866,7 +50899,7 @@
     </row>
     <row r="205" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="91" t="s">
-        <v>897</v>
+        <v>900</v>
       </c>
       <c r="B205" s="91"/>
       <c r="C205" s="91"/>
@@ -50915,7 +50948,7 @@
       <c r="AL205" s="93"/>
       <c r="AM205" s="93"/>
       <c r="AN205" s="93" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="AO205" s="93"/>
       <c r="AP205" s="93"/>
@@ -50975,7 +51008,7 @@
     </row>
     <row r="206" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="80" t="s">
-        <v>899</v>
+        <v>902</v>
       </c>
       <c r="B206" s="80"/>
       <c r="C206" s="80"/>
@@ -51234,7 +51267,7 @@
     </row>
     <row r="207" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A207" s="207" t="s">
-        <v>900</v>
+        <v>903</v>
       </c>
       <c r="B207" s="207"/>
       <c r="C207" s="207"/>
@@ -51283,7 +51316,7 @@
       <c r="AL207" s="93"/>
       <c r="AM207" s="93"/>
       <c r="AN207" s="93" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="AO207" s="93"/>
       <c r="AP207" s="93"/>
@@ -51343,7 +51376,7 @@
     </row>
     <row r="208" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A208" s="109" t="s">
-        <v>902</v>
+        <v>905</v>
       </c>
       <c r="B208" s="109"/>
       <c r="C208" s="109"/>
@@ -51602,7 +51635,7 @@
     </row>
     <row r="209" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="13" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="B209" s="13"/>
       <c r="C209" s="13"/>
@@ -51711,7 +51744,7 @@
     </row>
     <row r="210" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="109" t="s">
-        <v>904</v>
+        <v>907</v>
       </c>
       <c r="B210" s="109"/>
       <c r="C210" s="109"/>
@@ -51970,7 +52003,7 @@
     </row>
     <row r="211" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A211" s="13" t="s">
-        <v>905</v>
+        <v>908</v>
       </c>
       <c r="B211" s="13"/>
       <c r="C211" s="13"/>
@@ -52019,7 +52052,7 @@
       <c r="AL211" s="93"/>
       <c r="AM211" s="93"/>
       <c r="AN211" s="93" t="s">
-        <v>906</v>
+        <v>909</v>
       </c>
       <c r="AO211" s="93"/>
       <c r="AP211" s="93"/>
@@ -52079,7 +52112,7 @@
     </row>
     <row r="212" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="109" t="s">
-        <v>907</v>
+        <v>910</v>
       </c>
       <c r="B212" s="109"/>
       <c r="C212" s="109"/>
@@ -52338,7 +52371,7 @@
     </row>
     <row r="213" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A213" s="13" t="s">
-        <v>908</v>
+        <v>911</v>
       </c>
       <c r="B213" s="13"/>
       <c r="C213" s="13"/>
@@ -52387,7 +52420,7 @@
       <c r="AL213" s="93"/>
       <c r="AM213" s="93"/>
       <c r="AN213" s="93" t="s">
-        <v>909</v>
+        <v>912</v>
       </c>
       <c r="AO213" s="93"/>
       <c r="AP213" s="93"/>
@@ -52447,7 +52480,7 @@
     </row>
     <row r="214" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A214" s="80" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
       <c r="B214" s="80"/>
       <c r="C214" s="80"/>
@@ -52706,7 +52739,7 @@
     </row>
     <row r="215" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A215" s="91" t="s">
-        <v>911</v>
+        <v>914</v>
       </c>
       <c r="B215" s="91"/>
       <c r="C215" s="91"/>
@@ -52755,7 +52788,7 @@
       <c r="AL215" s="93"/>
       <c r="AM215" s="93"/>
       <c r="AN215" s="93" t="s">
-        <v>912</v>
+        <v>915</v>
       </c>
       <c r="AO215" s="93"/>
       <c r="AP215" s="93"/>
@@ -52815,7 +52848,7 @@
     </row>
     <row r="216" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="80" t="s">
-        <v>913</v>
+        <v>916</v>
       </c>
       <c r="B216" s="80"/>
       <c r="C216" s="80"/>
@@ -53074,7 +53107,7 @@
     </row>
     <row r="217" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="91" t="s">
-        <v>914</v>
+        <v>917</v>
       </c>
       <c r="B217" s="91"/>
       <c r="C217" s="91"/>
@@ -53123,7 +53156,7 @@
       <c r="AL217" s="93"/>
       <c r="AM217" s="93"/>
       <c r="AN217" s="93" t="s">
-        <v>915</v>
+        <v>918</v>
       </c>
       <c r="AO217" s="93"/>
       <c r="AP217" s="93"/>
@@ -53183,7 +53216,7 @@
     </row>
     <row r="218" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A218" s="80" t="s">
-        <v>916</v>
+        <v>919</v>
       </c>
       <c r="B218" s="80"/>
       <c r="C218" s="80"/>
@@ -53442,7 +53475,7 @@
     </row>
     <row r="219" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A219" s="207" t="s">
-        <v>917</v>
+        <v>920</v>
       </c>
       <c r="B219" s="207"/>
       <c r="C219" s="207"/>
@@ -53551,7 +53584,7 @@
     </row>
     <row r="220" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A220" s="109" t="s">
-        <v>918</v>
+        <v>921</v>
       </c>
       <c r="B220" s="109"/>
       <c r="C220" s="109"/>
@@ -53810,12 +53843,12 @@
     </row>
     <row r="221" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A221" s="13" t="s">
-        <v>919</v>
+        <v>922</v>
       </c>
       <c r="B221" s="13"/>
       <c r="C221" s="13"/>
       <c r="D221" s="92" t="s">
-        <v>920</v>
+        <v>923</v>
       </c>
       <c r="E221" s="92"/>
       <c r="F221" s="92"/>
@@ -53859,7 +53892,7 @@
       <c r="AL221" s="93"/>
       <c r="AM221" s="93"/>
       <c r="AN221" s="93" t="s">
-        <v>921</v>
+        <v>924</v>
       </c>
       <c r="AO221" s="93"/>
       <c r="AP221" s="93"/>
@@ -53919,7 +53952,7 @@
     </row>
     <row r="222" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A222" s="80" t="s">
-        <v>922</v>
+        <v>925</v>
       </c>
       <c r="B222" s="80"/>
       <c r="C222" s="80"/>
@@ -54178,7 +54211,7 @@
     </row>
     <row r="223" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A223" s="207" t="s">
-        <v>923</v>
+        <v>926</v>
       </c>
       <c r="B223" s="207"/>
       <c r="C223" s="207"/>
@@ -54287,7 +54320,7 @@
     </row>
     <row r="224" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A224" s="109" t="s">
-        <v>924</v>
+        <v>927</v>
       </c>
       <c r="B224" s="109"/>
       <c r="C224" s="109"/>
@@ -54546,12 +54579,12 @@
     </row>
     <row r="225" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="13" t="s">
-        <v>925</v>
+        <v>928</v>
       </c>
       <c r="B225" s="13"/>
       <c r="C225" s="13"/>
       <c r="D225" s="92" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="E225" s="92"/>
       <c r="F225" s="92"/>
@@ -54595,7 +54628,7 @@
       <c r="AL225" s="93"/>
       <c r="AM225" s="93"/>
       <c r="AN225" s="93" t="s">
-        <v>927</v>
+        <v>930</v>
       </c>
       <c r="AO225" s="93"/>
       <c r="AP225" s="93"/>
@@ -54655,7 +54688,7 @@
     </row>
     <row r="226" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="80" t="s">
-        <v>928</v>
+        <v>931</v>
       </c>
       <c r="B226" s="80"/>
       <c r="C226" s="80"/>
@@ -54914,7 +54947,7 @@
     </row>
     <row r="227" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A227" s="207" t="s">
-        <v>929</v>
+        <v>932</v>
       </c>
       <c r="B227" s="207"/>
       <c r="C227" s="207"/>
@@ -54963,7 +54996,7 @@
       <c r="AL227" s="93"/>
       <c r="AM227" s="93"/>
       <c r="AN227" s="93" t="s">
-        <v>930</v>
+        <v>933</v>
       </c>
       <c r="AO227" s="93"/>
       <c r="AP227" s="93"/>
@@ -55023,7 +55056,7 @@
     </row>
     <row r="228" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A228" s="109" t="s">
-        <v>931</v>
+        <v>934</v>
       </c>
       <c r="B228" s="109"/>
       <c r="C228" s="109"/>
@@ -55282,7 +55315,7 @@
     </row>
     <row r="229" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="13" t="s">
-        <v>932</v>
+        <v>935</v>
       </c>
       <c r="B229" s="13"/>
       <c r="C229" s="13"/>
@@ -55391,7 +55424,7 @@
     </row>
     <row r="230" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="109" t="s">
-        <v>933</v>
+        <v>936</v>
       </c>
       <c r="B230" s="109"/>
       <c r="C230" s="109"/>
@@ -55650,12 +55683,12 @@
     </row>
     <row r="231" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="13" t="s">
-        <v>934</v>
+        <v>937</v>
       </c>
       <c r="B231" s="13"/>
       <c r="C231" s="13"/>
       <c r="D231" s="92" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="E231" s="92"/>
       <c r="F231" s="92"/>
@@ -55699,7 +55732,7 @@
       <c r="AL231" s="93"/>
       <c r="AM231" s="93"/>
       <c r="AN231" s="93" t="s">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="AO231" s="93"/>
       <c r="AP231" s="93"/>
@@ -55759,7 +55792,7 @@
     </row>
     <row r="232" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="80" t="s">
-        <v>937</v>
+        <v>940</v>
       </c>
       <c r="B232" s="80"/>
       <c r="C232" s="80"/>
@@ -56018,7 +56051,7 @@
     </row>
     <row r="233" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A233" s="207" t="s">
-        <v>938</v>
+        <v>941</v>
       </c>
       <c r="B233" s="207"/>
       <c r="C233" s="207"/>
@@ -56067,7 +56100,7 @@
       <c r="AL233" s="93"/>
       <c r="AM233" s="93"/>
       <c r="AN233" s="93" t="s">
-        <v>939</v>
+        <v>942</v>
       </c>
       <c r="AO233" s="93"/>
       <c r="AP233" s="93"/>
@@ -56127,7 +56160,7 @@
     </row>
     <row r="234" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A234" s="109" t="s">
-        <v>940</v>
+        <v>943</v>
       </c>
       <c r="B234" s="109"/>
       <c r="C234" s="109"/>
@@ -56386,7 +56419,7 @@
     </row>
     <row r="235" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="13" t="s">
-        <v>941</v>
+        <v>944</v>
       </c>
       <c r="B235" s="13"/>
       <c r="C235" s="13"/>
@@ -56495,7 +56528,7 @@
     </row>
     <row r="236" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A236" s="109" t="s">
-        <v>942</v>
+        <v>945</v>
       </c>
       <c r="B236" s="109"/>
       <c r="C236" s="109"/>
@@ -56754,12 +56787,12 @@
     </row>
     <row r="237" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="13" t="s">
-        <v>943</v>
+        <v>946</v>
       </c>
       <c r="B237" s="13"/>
       <c r="C237" s="13"/>
       <c r="D237" s="92" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="E237" s="92"/>
       <c r="F237" s="92"/>
@@ -56803,7 +56836,7 @@
       <c r="AL237" s="93"/>
       <c r="AM237" s="93"/>
       <c r="AN237" s="93" t="s">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="AO237" s="93"/>
       <c r="AP237" s="93"/>
@@ -56863,7 +56896,7 @@
     </row>
     <row r="238" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="80" t="s">
-        <v>944</v>
+        <v>947</v>
       </c>
       <c r="B238" s="80"/>
       <c r="C238" s="80"/>
@@ -57122,7 +57155,7 @@
     </row>
     <row r="239" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A239" s="207" t="s">
-        <v>945</v>
+        <v>948</v>
       </c>
       <c r="B239" s="207"/>
       <c r="C239" s="207"/>
@@ -57171,7 +57204,7 @@
       <c r="AL239" s="93"/>
       <c r="AM239" s="93"/>
       <c r="AN239" s="93" t="s">
-        <v>946</v>
+        <v>949</v>
       </c>
       <c r="AO239" s="93"/>
       <c r="AP239" s="93"/>
@@ -57231,7 +57264,7 @@
     </row>
     <row r="240" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="80" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="B240" s="80"/>
       <c r="C240" s="80"/>
@@ -57490,7 +57523,7 @@
     </row>
     <row r="241" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="91" t="s">
-        <v>948</v>
+        <v>951</v>
       </c>
       <c r="B241" s="91"/>
       <c r="C241" s="91"/>
@@ -57599,7 +57632,7 @@
     </row>
     <row r="242" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A242" s="80" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
       <c r="B242" s="80"/>
       <c r="C242" s="80"/>
@@ -57858,7 +57891,7 @@
     </row>
     <row r="243" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A243" s="207" t="s">
-        <v>950</v>
+        <v>953</v>
       </c>
       <c r="B243" s="207"/>
       <c r="C243" s="207"/>
@@ -57907,7 +57940,7 @@
       <c r="AL243" s="93"/>
       <c r="AM243" s="93"/>
       <c r="AN243" s="93" t="s">
-        <v>951</v>
+        <v>954</v>
       </c>
       <c r="AO243" s="93"/>
       <c r="AP243" s="93"/>
@@ -57949,7 +57982,7 @@
       <c r="BZ243" s="93"/>
       <c r="CA243" s="93"/>
       <c r="CB243" s="202" t="s">
-        <v>952</v>
+        <v>955</v>
       </c>
       <c r="CC243" s="202"/>
       <c r="CD243" s="202"/>
@@ -57967,7 +58000,7 @@
     </row>
     <row r="244" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A244" s="80" t="s">
-        <v>953</v>
+        <v>956</v>
       </c>
       <c r="B244" s="80"/>
       <c r="C244" s="80"/>
@@ -58226,12 +58259,12 @@
     </row>
     <row r="245" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A245" s="207" t="s">
-        <v>954</v>
+        <v>957</v>
       </c>
       <c r="B245" s="207"/>
       <c r="C245" s="207"/>
       <c r="D245" s="92" t="s">
-        <v>955</v>
+        <v>958</v>
       </c>
       <c r="E245" s="92"/>
       <c r="F245" s="92"/>
@@ -58275,7 +58308,7 @@
       <c r="AL245" s="93"/>
       <c r="AM245" s="93"/>
       <c r="AN245" s="93" t="s">
-        <v>951</v>
+        <v>954</v>
       </c>
       <c r="AO245" s="93"/>
       <c r="AP245" s="93"/>
@@ -58317,7 +58350,7 @@
       <c r="BZ245" s="93"/>
       <c r="CA245" s="93"/>
       <c r="CB245" s="202" t="s">
-        <v>952</v>
+        <v>955</v>
       </c>
       <c r="CC245" s="202"/>
       <c r="CD245" s="202"/>
@@ -58335,7 +58368,7 @@
     </row>
     <row r="246" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="80" t="s">
-        <v>956</v>
+        <v>959</v>
       </c>
       <c r="B246" s="80"/>
       <c r="C246" s="80"/>
@@ -58593,7 +58626,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2013">
+  <mergeCells count="2016">
     <mergeCell ref="A1:C3"/>
     <mergeCell ref="CK1:CL1"/>
     <mergeCell ref="CM1:CO1"/>
@@ -60254,7 +60287,9 @@
     <mergeCell ref="AH157:AM157"/>
     <mergeCell ref="AN157:CA157"/>
     <mergeCell ref="CB157:CG157"/>
+    <mergeCell ref="CQ157:CS157"/>
     <mergeCell ref="A158:C158"/>
+    <mergeCell ref="CQ158:CS158"/>
     <mergeCell ref="A159:C159"/>
     <mergeCell ref="D159:H159"/>
     <mergeCell ref="I159:N159"/>
@@ -60262,6 +60297,7 @@
     <mergeCell ref="AH159:AM159"/>
     <mergeCell ref="AN159:CA159"/>
     <mergeCell ref="CB159:CG159"/>
+    <mergeCell ref="CQ159:CS159"/>
     <mergeCell ref="A160:C160"/>
     <mergeCell ref="A161:C161"/>
     <mergeCell ref="D161:H161"/>

</xml_diff>